<commit_message>
Reload Temples and Persons and Show worship days
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/храмы.xlsx
+++ b/loadDatabase/religion/храмы.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,12 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$J$1</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="682">
   <si>
     <t>название</t>
   </si>
@@ -2296,20 +2293,339 @@
     <t>10в</t>
   </si>
   <si>
+    <t xml:space="preserve">17.04. 1636 </t>
+  </si>
+  <si>
     <t xml:space="preserve">06.10.1885 </t>
   </si>
   <si>
     <t xml:space="preserve">14.09.1857 </t>
   </si>
   <si>
-    <t xml:space="preserve">17.04.1636 </t>
+    <t>Киево-Печерская лавра</t>
+  </si>
+  <si>
+    <t>50°25′56″ с. ш. 30°33′44″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/f/fb/%D0%9B%D0%B0%D0%B2%D1%80%D0%B0.jpg/1280px-%D0%9B%D0%B0%D0%B2%D1%80%D0%B0.jpg </t>
+  </si>
+  <si>
+    <t>Киев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Храм_Василия_Блаженного </t>
+  </si>
+  <si>
+    <t>Епископ Ермоген (Голубев)</t>
+  </si>
+  <si>
+    <t>Свя́то-Успе́нская Ки́ево-Пече́рская ла́вра (укр. Свято-Успенська Києво-Печерська лавра) — один из первых по времени основания монастырей Киевской Руси. Одна из важнейших православных святынь, третий Удел Богородицы. Печерский монастырь был основан в 1051 году при Ярославе Мудром монахом Антонием, родом из Любеча, и его учеником Феодосием. В 1688 году монастырь получил статус лавры и стал «ставропигионом царским и патриаршим Московским»; в 1786 году лавра была подчинена киевскому митрополиту, который стал её священноархимандритом. В настоящее время Нижняя лавра находится в ведении Украинской православной церкви (Московского патриархата), а Верхняя лавра — в ведении Киево-Печерского историко-культурного заповедника.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Киево-Печерская_лавра </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://mitropolia.kiev.ua </t>
+  </si>
+  <si>
+    <t>Благовещенский собор</t>
+  </si>
+  <si>
+    <t>49°59′25″ с. ш. 36°13′27″ в. д.</t>
+  </si>
+  <si>
+    <t>Харьков</t>
+  </si>
+  <si>
+    <t>https://ua.igotoworld.com/frontend/webcontent/websites/1/images/gallery/9098_800x600_11996.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.eparchia.kharkov.ua </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Благовещенский_собор_(Харьков) </t>
+  </si>
+  <si>
+    <t>Свящ. Иоанн Матвеев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Первая церковь во имя Благовещения Пресвятой Богородицы основана около 1655 г., одновременно с Николаевской и Рождественской.  Бурное развитие поселения дало толчок к расширению прихода: согласно Куряжским актам 1720 г. в штате церкви находятся уже двое священников. После крупного пожара в 1738 г. восстановлена в том же виде. В 1789 году был заложен новый каменный однокупольный храм в стиле раннего классицизма по проекту П. А. Ярославского, освящённый 8 сентября 1794 года Торжественная закладка новой церкви была совершена 2 октября 1888 года рядом со старым храмом, действовавшим во время двенадцатилетнего строительства.
+ </t>
+  </si>
+  <si>
+    <t>Свято-Владимирский собор</t>
+  </si>
+  <si>
+    <t>Луганск</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/c/c9/%D0%92%D0%BE%D0%BB%D0%BE%D0%B4%D0%B8%D0%BC%D0%B8%D1%80%D1%81%D1%8C%D0%BA%D0%B8%D0%B9_%D0%BA%D0%B0%D1%84%D0%B5%D0%B4%D1%80%D0%B0%D0%BB%D1%8C%D0%BD%D1%8B%D0%B9_%D1%81%D0%BE%D0%B1%D0%BE%D1%80_%28%D0%9B%D1%83%D0%B3%D0%B0%D0%BD%D1%81%D1%8C%D0%BA%29.JPG/1280px-%D0%92%D0%BE%D0%BB%D0%BE%D0%B4%D0%B8%D0%BC%D0%B8%D1%80%D1%81%D1%8C%D0%BA%D0%B8%D0%B9_%D0%BA%D0%B0%D1%84%D0%B5%D0%B4%D1%80%D0%B0%D0%BB%D1%8C%D0%BD%D1%8B%D0%B9_%D1%81%D0%BE%D0%B1%D0%BE%D1%80_%28%D0%9B%D1%83%D0%B3%D0%B0%D0%BD%D1%81%D1%8C%D0%BA%29.JPG  </t>
+  </si>
+  <si>
+    <t>48°33′48″ с. ш. 39°21′02″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lugansk.church.ua </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Свято-Владимирский_собор_(Луганск) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Протоиерей Владимир Конончук </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Владимирский собор — православный собор в Луганске, являющийся на сегодняшний день самым крупным культовым сооружением юго-восточной Украины. Собор вмещает около 3 тысяч прихожан. При соборе расположен Луганский богословский университет в честь Архистратига Михаила (ранее — Луганская духовная семинария). 9 апреля 1993 года состоялась торжественная церемония освящения места возведения будущего собора Митрополитом Киевским и всея Украины, Предстоятелем Украинской Православной Церкви Блаженнейшим Владимиром и Архиепископом Луганским и Старобельским Иоанникием. В мае 1995 года — вынут первый ковш грунта из котлована под фундамент собора. </t>
+  </si>
+  <si>
+    <t>Спасо-Преображенский кафедральный собор</t>
+  </si>
+  <si>
+    <t>48°00′40″ с. ш. 37°48′18″ в. д.</t>
+  </si>
+  <si>
+    <t>Донецк</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/a/af/DonetskCathedral.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://donetsk.church.ua </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Спасо-Преображенский_кафедральный_собор_(Донецк) </t>
+  </si>
+  <si>
+    <t>Митрополит Донецкий и Мариупольский Иларион</t>
+  </si>
+  <si>
+    <t>Свято-Преображенский собор (Спасо-Преображенским назывался храм в Юзовке) — кафедральный православный храм в Донецке в честь Преображения Господня, главный храм Донецкой и Мариупольской епархии Украинской Православной Церкви Московского патриархата (Московский патриархат). Нынешнее здание построено в 1990-х — 2000-х годах по образцу одноимённой церкви, разрушенной в 1931 году.</t>
+  </si>
+  <si>
+    <t>Троицкий собор</t>
+  </si>
+  <si>
+    <t>51°28′38″ с. ш. 31°16′49″ в. д.</t>
+  </si>
+  <si>
+    <t>Чернигов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/1/15/Chernigov_Holy_Trinity_Cathedral.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://orthodox.com.ua </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Троицкий_собор_(Чернигов) </t>
+  </si>
+  <si>
+    <t>Свято-Троицкий кафедральный собор в Чернигове — кафедральный собор Черниговской епархии Украинской Православной Церкви. Ранее входил в комплекс Троице-Ильинского монастыря. Построен в стиле украинского барокко на средства полковника Василия Дунина и гетьмана Ивана Мазепы в 1679-1689 гг. Собор имеет статус кафедрального. В основу Троицкого собора положен тип крестовокупольного храма. По обеим сторонам западного фасада имеются две башни, которые увенчаны высоким верхом.</t>
+  </si>
+  <si>
+    <t>Собор Сошествия Святого Духа</t>
+  </si>
+  <si>
+    <t>Минкс</t>
+  </si>
+  <si>
+    <t>53°54′18″ с. ш. 27°33′22″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/6/6e/Holy_Spirit_Cathedral_in_Minsk.jpg/1280px-Holy_Spirit_Cathedral_in_Minsk.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.church.by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Собор_Сошествия_Святого_Духа_(Минск) </t>
+  </si>
+  <si>
+    <t>Кафедральный собор Сошествия Святого Духа — главный храм Белорусского экзархата Русской Православной церкви. Бывший костёл монастыря бернардинок; одна из главных достопримечательностей Верхнего города. История собора начинается в 1633—1642 годах, когда было построено здание, служившее храмом католического монастыря бернардинок. В 1741 году здание было разрушено пожаром, который стал причиной реконструкции монастыря. В 1852 году монастырь был переведён в Несвиж. С 1860 года прежний костел стал православным храмом.</t>
+  </si>
+  <si>
+    <t>Храм Воскресения Христова</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/0/01/Hram_Voskresenija_Hristova_20070505.jpg/800px-Hram_Voskresenija_Hristova_20070505.jpg </t>
+  </si>
+  <si>
+    <t>53°57′22″ с. ш. 27°36′12″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.church.by  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Храм_Воскресения_Христова_(Минск) </t>
+  </si>
+  <si>
+    <t>протоиерей Георгий Арбузов</t>
+  </si>
+  <si>
+    <t>Храм Воскресения Христова — православный храм в микрорайоне Зеленый Луг Минска. Настоятелем храма является протоиерей Георгий Арбузов. Белоснежный пятиглавый храм Воскресения Христова состоит из двух церквей: нижней — криптовой, во имя белорусского святого, праведного Иоанна Кормянского, где хранится частица его мощей (церковь освящена в мае 2000 года), и верхней — в честь Воскресения Христова. При приходе действует Сестричество милосердия во имя святых Царственных страстотерпцев и богословское Братство во имя Иоанна Предтечи. Работают иконописно-реставрационная мастерская, мастерская по швейному делу, кружки по интересам для детей и молодежи, есть библиотека.</t>
+  </si>
+  <si>
+    <t>Свято-Симеоновский собор</t>
+  </si>
+  <si>
+    <t>Брест</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/4/45/%D0%A1%D1%8C%D0%B2%D1%8F%D1%82%D0%B0-%D0%A1%D1%96%D0%BC%D1%8F%D0%BE%D0%BD%D0%B0%D1%9E%D1%81%D0%BA%D1%96_%D1%81%D0%B0%D0%B1%D0%BE%D1%80_%28%D0%91%D0%B5%D1%80%D0%B0%D1%81%D1%8C%D1%86%D0%B5%29_%D0%97%D0%B0%D0%B4%D0%BD%D1%96_%D0%B1%D0%BE%D0%BA.jpg/1280px-%D0%A1%D1%8C%D0%B2%D1%8F%D1%82%D0%B0-%D0%A1%D1%96%D0%BC%D1%8F%D0%BE%D0%BD%D0%B0%D1%9E%D1%81%D0%BA%D1%96_%D1%81%D0%B0%D0%B1%D0%BE%D1%80_%28%D0%91%D0%B5%D1%80%D0%B0%D1%81%D1%8C%D1%86%D0%B5%29_%D0%97%D0%B0%D0%B4%D0%BD%D1%96_%D0%B1%D0%BE%D0%BA.jpg </t>
+  </si>
+  <si>
+    <t>52°05′07″ с. ш. 23°41′24″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Свято-Симеоновский_собор_(Брест) </t>
+  </si>
+  <si>
+    <t>Свя́то-Симео́новский собо́р, Собо́р Симео́на Сто́лпника — православный собор в Бресте (Белоруссия). Является памятником архитектуры русско-византийского стиля. Кафедральный собор Брестской и Кобринской епархии. В 1846 году был утверждён первый проект строительства храма. Впоследствии он был значительно упрощён, так как на последовавших торгах покупателей для подряда по строительству храма не было найдено, что вынудило принять решение вести работы лишь в пределах выделенной правительством суммы. Новый проект, согласно докладу генерал-адъютанта графа Клейнмихеля, утвердили 15 апреля 1854 года</t>
+  </si>
+  <si>
+    <t>Свято-Духов монастырь</t>
+  </si>
+  <si>
+    <t>Витебск</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/42/Sv-Duhov-monastery_Vitebsk.jpg/1280px-Sv-Duhov-monastery_Vitebsk.jpg</t>
+  </si>
+  <si>
+    <t>55°11′42″ с. ш. 30°12′06″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vitprav.by </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Свято-Духов_монастырь_(Витебск)</t>
+  </si>
+  <si>
+    <t>Свято-Духов монастырь (белор. Свята-Духаўскі манастыр) — православный монастырь в Витебске (Белоруссия). Монастырь основан в конце 1380-х годов витебской княгиней Иулианией Александровной, женой Великого князя Литовского Ольгерда, который выстроил главный храм обители — церковь Святого Духа. Примерно в 1392—1393 годах она приняла в монастыре схиму под именем Марфы. По легенде, княгиня Ульяния провела в монастыре при Свято-Духовской церкви последние годы жизни и была здесь похоронена. В 1618 году возник вопрос о превращении монастыря в униатско-базилианский кляштор. Униаты обосновались здесь после войны России с Речью Посполитой (1654—1667). В 1839 году Свято-Духов монастырь вновь стал православным.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.orthos.org </t>
+  </si>
+  <si>
+    <t>Борисоглебская церковь</t>
+  </si>
+  <si>
+    <t>Гродно</t>
+  </si>
+  <si>
+    <t>53°40′42″ с. ш. 23°49′07″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/f/f5/%D0%93%D1%80%D0%BE%D0%B4%D0%BD%D0%B0._%D0%9A%D0%B0%D0%BB%D0%BE%D0%B6%D1%81%D0%BA%D0%B0%D1%8F_%D1%86%D0%B0%D1%80%D0%BA%D0%B2%D0%B0_2.JPG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Борисоглебская_церковь_(Гродно) </t>
+  </si>
+  <si>
+    <t>Борисогле́бская це́рковь, Коложская церковь или просто Коло́жа — одно из сохранившихся архитектурных сооружений Белоруссии периода Древней Руси. Единственный сохранившийся (в искажённом виде) памятник чёрнорусского зодчества. Расположена на высоком берегу реки Неман. Предположительно, церковь была построена во время правления гродненских князей Бориса и Глеба Всеволодковичей (первый умер до 1166, второй — в 1170) и освящена в честь их небесных покровителей, Бориса и Глеба. По другой версии — храм возведён в 1180-е годы детьми Бориса и Глеба. Возведение храма осуществлялось на месте урочища Коложань (название «коложань, коложень» обозначает место, где бьют многочисленные родники), которое почиталось окрестными язычниками. Согласно другим исследованиям, название урочища происходит от жителей псковской крепости Коложа, взятых в плен великим князем Витовтом во время его нападения на Псков в 1406 году.</t>
+  </si>
+  <si>
+    <t>Полоцк</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/c/c2/Bog-2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55°29′02″ с. ш. 28°46′07″ в. д. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Богоявленский_собор_(Полоцк) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eparhia992.by </t>
+  </si>
+  <si>
+    <t>Свя́то-Богоявле́нский собо́р (белор. Свята-Богаяўленскі сабор) — православный кафедральный собор в стиле барокко в Полоцке, часть комплекса Свято-Богоявленского монастыря, памятник архитектуры XVIII века. Действующий кафедральный собор Полоцкой и Глубокской епархии. В 1761 году монахи Свято-Богоявленского монастыря начали строительство каменного собора. 5 августа 1777 года он был освящён.</t>
+  </si>
+  <si>
+    <t>Светицховели</t>
+  </si>
+  <si>
+    <t>41°50′31″ с. ш. 44°43′16″ в. д.</t>
+  </si>
+  <si>
+    <t>Мцхета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/6/61/Svetitskhoveli_Cathedral_in_Georgia%2C_Europe.jpg </t>
+  </si>
+  <si>
+    <t>4в</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://patriarchate.ge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Светицховели </t>
+  </si>
+  <si>
+    <t>Светицховели (груз. სვეტიცხოველი — животворящий столп) — кафедральный патриарший храм Грузинской православной церкви в честь двенадцати Апостолов, в городе Мцхета, который на протяжении тысячелетия являлся главным собором всей Грузии. С 1994 г. памятник Всемирного наследия. Среди сохранившихся исторических сооружений Светицховели является самым большим в Грузии. На протяжении веков является центром христианской Грузии. Ещё в IV веке принявший христианство царь Мириан III по совету равноапостольной Нины выстроил на месте современного храма первую в Грузии деревянную церковь, которая не дошла до сегодняшних дней.</t>
+  </si>
+  <si>
+    <t>Цминда Самеба</t>
+  </si>
+  <si>
+    <t>41°41′51″ с. ш. 44°49′00″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/0/04/2014_Tbilisi%2C_Sob%C3%B3r_Tr%C3%B3jcy_%C5%9Awi%C4%99tej_%2817%29.jpg/1280px-2014_Tbilisi%2C_Sob%C3%B3r_Tr%C3%B3jcy_%C5%9Awi%C4%99tej_%2817%29.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Цминда_Самеба </t>
+  </si>
+  <si>
+    <t>Цми́нда Са́меба (груз. წმინდა სამება — «Пресвятая Троица») — второй после Светицховели кафедральный собор Грузинской православной церкви, который находится в Тбилиси, на холме Св. Ильи (левый берег Куры). В соборе 13 престолов; нижний храм в честь Благовещения Пресвятой Богородицы; отдельно стоит звонница. Строительство нового собора было запланировано в 1989 году в связи с празднованием 1500-летия автокефалии Грузинской церкви и в ознаменование 2000-летия христианства.</t>
+  </si>
+  <si>
+    <t>Собор Влахернской иконы Божией Матери</t>
+  </si>
+  <si>
+    <t>42°30′43″ с. ш. 41°52′28″ в. д.</t>
+  </si>
+  <si>
+    <t>Зугдиди</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/e/e7/Zugdidi81.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Собор_Влахернской_иконы_Божией_Матери </t>
+  </si>
+  <si>
+    <t>Собор Влахернской иконы Божией Матери(груз. ზუგდიდის ვლაქერნის ყოვლადწმიდა ღმრთისმშობლის ხატის სახელობის საკათედრო ტაძარი) — кафедральный храм Грузинской православной церкви в Зугдиди. Центр Зугдидской и Цаишской епархии. Эквтиме Такаишвили отмечает, что «Церковь нового Зугдиди построена из камня, грузинского стиля, при правлении Левана V Дадиани, строительство началось в 1825 году, а окончилось в 1830 году». Деньги на строительство выделил российский император Александр I, он же вернул один из списков Влахернской иконы Божией Матери, которая по преданию не раз спасала Константинополь от нашествия врагов.</t>
+  </si>
+  <si>
+    <t>Тимотесубани</t>
+  </si>
+  <si>
+    <t>41°48′38″ с. ш. 43°31′05″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/1/18/Timotesubani_Monastery_%28photo_by_Mamuka_Chduneli%29.jpg/800px-Timotesubani_Monastery_%28photo_by_Mamuka_Chduneli%29.jpg </t>
+  </si>
+  <si>
+    <t>Тимотесубани (груз. ტიმოთესუბანი), официально Храм Успения Пресвятой Богородицы, находится в Боржомском районе Грузии, 18 километрах от города Боржоми, на правом берегу реки Гуджарула. Относится к Боржомско-Бакурианской епархии. Храм построен на развалинах древнего монастыря владетелем тех мест,святым мучеником,князем Шалвой Торели-Ахалцихели,национальным героем Грузии. Начало строительства датируется 1195 годом и завершено в 1215 году.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Тимотесубани_(храм)</t>
+  </si>
+  <si>
+    <t>Минск</t>
+  </si>
+  <si>
+    <t>Тбилиси</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2327,6 +2643,20 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2357,20 +2687,8 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2390,6 +2708,26 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2452,7 +2790,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2484,10 +2822,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2519,7 +2856,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2695,20 +3031,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="20.7109375" style="5"/>
+    <col min="5" max="5" width="20.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.95" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +3057,7 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
@@ -2737,165 +3073,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="11">
         <v>1637</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" s="14" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="12">
         <v>1799</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.95" customHeight="1">
       <c r="A4" t="s">
         <v>348</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="1">
         <v>1868</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.95" customHeight="1">
       <c r="A5" t="s">
         <v>351</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="1">
         <v>1889</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.95" customHeight="1">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>533</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="1">
         <v>1877</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.95" customHeight="1">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>534</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.95" customHeight="1">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="1">
         <v>1995</v>
       </c>
       <c r="F8" t="s">
@@ -2907,2208 +3243,2208 @@
       <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.95" customHeight="1">
       <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>535</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="1">
         <v>2009</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18.95" customHeight="1">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.95" customHeight="1">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <v>40268</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.95" customHeight="1">
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="1">
         <v>2002</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18.95" customHeight="1">
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.95" customHeight="1">
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="1">
         <v>1841</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18.95" customHeight="1">
       <c r="A15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="1">
         <v>1863</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="18.95" customHeight="1">
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="1">
         <v>1898</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="18.95" customHeight="1">
       <c r="A17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="1">
         <v>1915</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="18.95" customHeight="1">
       <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="1">
         <v>2001</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="18.95" customHeight="1">
       <c r="A19" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="1">
         <v>2006</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="18.95" customHeight="1">
       <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="8">
         <v>36646</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="18.95" customHeight="1">
       <c r="A21" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="1">
         <v>1997</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="18.95" customHeight="1">
       <c r="A22" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="1">
         <v>2014</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="18.95" customHeight="1">
       <c r="A23" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="1">
         <v>1811</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="18.95" customHeight="1">
       <c r="A24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="1">
         <v>1843</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="18.95" customHeight="1">
       <c r="A25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="1">
         <v>1870</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="18.95" customHeight="1">
       <c r="A26" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="1">
         <v>1867</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="18.95" customHeight="1">
       <c r="A27" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="1">
         <v>2002</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="18.95" customHeight="1">
       <c r="A28" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="1">
         <v>1955</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="18.95" customHeight="1">
       <c r="A29" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="1">
         <v>1905</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="18.95" customHeight="1">
       <c r="A30" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="1">
         <v>1904</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="18.95" customHeight="1">
       <c r="A31" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="1">
         <v>1872</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="18.95" customHeight="1">
       <c r="A32" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="1">
         <v>1800</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="18.95" customHeight="1">
       <c r="A33" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="1">
         <v>1918</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="18.95" customHeight="1">
       <c r="A34" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="1">
         <v>1894</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="3" t="s">
         <v>134</v>
       </c>
       <c r="G34" t="s">
         <v>135</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A35" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="1">
         <v>1885</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="10" t="s">
+      <c r="G35" s="1"/>
+      <c r="H35" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="I35" s="10" t="s">
+      <c r="I35" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="10" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="1">
         <v>1903</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I36" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="10" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="F37" s="9" t="s">
+      <c r="E37" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="10" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="10" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="1">
         <v>1896</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="10" t="s">
+      <c r="G38" s="1"/>
+      <c r="H38" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="10" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="1">
         <v>2018</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="10" t="s">
+      <c r="G39" s="1"/>
+      <c r="H39" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="10" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="1">
         <v>1838</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="10" t="s">
+      <c r="G40" s="1"/>
+      <c r="H40" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="I40" s="10" t="s">
+      <c r="I40" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="10" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="1">
         <v>1888</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="10" t="s">
+      <c r="G41" s="1"/>
+      <c r="H41" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I41" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="1">
         <v>1857</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F42" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5" t="s">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I42" s="10" t="s">
+      <c r="I42" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="1">
         <v>1817</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="10" t="s">
+      <c r="G43" s="1"/>
+      <c r="H43" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="I43" s="10" t="s">
+      <c r="I43" s="6" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="1">
         <v>2002</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="10" t="s">
+      <c r="G44" s="1"/>
+      <c r="H44" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="I44" s="10" t="s">
+      <c r="I44" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="1"/>
+      <c r="C45" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="1">
         <v>2001</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="10" t="s">
+      <c r="G45" s="1"/>
+      <c r="H45" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I45" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="1"/>
+      <c r="C46" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="1">
         <v>1714</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="10" t="s">
+      <c r="G46" s="1"/>
+      <c r="H46" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="I46" s="10" t="s">
+      <c r="I46" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A47" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="10" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="1">
         <v>1855</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="10" t="s">
+      <c r="G47" s="1"/>
+      <c r="H47" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I47" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A48" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="10" t="s">
+      <c r="B48" s="1"/>
+      <c r="C48" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="1">
         <v>1906</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="10" t="s">
+      <c r="G48" s="1"/>
+      <c r="H48" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="I48" s="10" t="s">
+      <c r="I48" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A49" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="1"/>
+      <c r="C49" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="1">
         <v>1860</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="10" t="s">
+      <c r="G49" s="1"/>
+      <c r="H49" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="I49" s="10" t="s">
+      <c r="I49" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A50" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="10" t="s">
+      <c r="B50" s="1"/>
+      <c r="C50" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="1">
         <v>2018</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="10" t="s">
+      <c r="G50" s="1"/>
+      <c r="H50" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="I50" s="10" t="s">
+      <c r="I50" s="6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A51" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="10" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="1">
         <v>1822</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="G51" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H51" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="I51" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A52" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="10" t="s">
+      <c r="B52" s="1"/>
+      <c r="C52" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="1">
         <v>2009</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="1"/>
+      <c r="H52" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="I52" s="10" t="s">
+      <c r="I52" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A53" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="10" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="1">
         <v>2014</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="10" t="s">
+      <c r="G53" s="1"/>
+      <c r="H53" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="I53" s="10" t="s">
+      <c r="I53" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A54" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="10" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E54" s="8">
         <v>40860</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="10" t="s">
+      <c r="G54" s="1"/>
+      <c r="H54" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="I54" s="10" t="s">
+      <c r="I54" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="55" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A55" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="10" t="s">
+      <c r="B55" s="1"/>
+      <c r="C55" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E55" s="12">
+      <c r="E55" s="8">
         <v>41579</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="10" t="s">
+      <c r="G55" s="1"/>
+      <c r="H55" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="I55" s="10" t="s">
+      <c r="I55" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="56" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A56" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="10" t="s">
+      <c r="B56" s="1"/>
+      <c r="C56" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="12">
+      <c r="E56" s="8">
         <v>43033</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="10" t="s">
+      <c r="G56" s="1"/>
+      <c r="H56" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="I56" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A57" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="10" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="12">
+      <c r="E57" s="8">
         <v>43744</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="10" t="s">
+      <c r="G57" s="1"/>
+      <c r="H57" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="I57" s="6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A58" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="10" t="s">
+      <c r="B58" s="1"/>
+      <c r="C58" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E58" s="12">
+      <c r="E58" s="8">
         <v>43030</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="10" t="s">
+      <c r="G58" s="1"/>
+      <c r="H58" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="I58" s="10" t="s">
+      <c r="I58" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="10" t="s">
+      <c r="B59" s="1"/>
+      <c r="C59" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E59" s="12">
+      <c r="E59" s="8">
         <v>2116</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G59" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="H59" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="I59" s="10" t="s">
+      <c r="I59" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A60" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="10" t="s">
+      <c r="B60" s="1"/>
+      <c r="C60" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E60" s="12">
+      <c r="E60" s="8">
         <v>38951</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G60" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H60" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="I60" s="10" t="s">
+      <c r="I60" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A61" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="10" t="s">
+      <c r="B61" s="1"/>
+      <c r="C61" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E61" s="12">
+      <c r="E61" s="8">
         <v>41833</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="10" t="s">
+      <c r="G61" s="1"/>
+      <c r="H61" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="I61" s="10" t="s">
+      <c r="I61" s="6" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A62" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="10" t="s">
+      <c r="B62" s="1"/>
+      <c r="C62" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="8">
         <v>36289</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="10" t="s">
+      <c r="G62" s="1"/>
+      <c r="H62" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="I62" s="10" t="s">
+      <c r="I62" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="18.95" customHeight="1">
       <c r="A63" t="s">
         <v>260</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="2" t="s">
         <v>512</v>
       </c>
       <c r="D63" t="s">
         <v>261</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="1">
         <v>1161</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="3" t="s">
         <v>262</v>
       </c>
       <c r="G63" t="s">
         <v>263</v>
       </c>
-      <c r="H63" s="6" t="s">
+      <c r="H63" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="I63" s="6" t="s">
+      <c r="I63" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="18.95" customHeight="1">
       <c r="A64" t="s">
         <v>266</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="2" t="s">
         <v>513</v>
       </c>
       <c r="D64" t="s">
         <v>261</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="1">
         <v>1194</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="H64" s="6" t="s">
+      <c r="H64" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="I64" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="18.95" customHeight="1">
       <c r="A65" t="s">
         <v>270</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="2" t="s">
         <v>514</v>
       </c>
       <c r="D65" t="s">
         <v>271</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="1">
         <v>1158</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H65" s="6" t="s">
+      <c r="H65" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="I65" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="18.95" customHeight="1">
       <c r="A66" t="s">
         <v>275</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="2" t="s">
         <v>515</v>
       </c>
       <c r="D66" t="s">
         <v>276</v>
       </c>
-      <c r="E66" s="5">
+      <c r="E66" s="1">
         <v>1222</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="3" t="s">
         <v>278</v>
       </c>
       <c r="G66" t="s">
         <v>277</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I66" s="6" t="s">
+      <c r="I66" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="18.95" customHeight="1">
       <c r="A67" t="s">
         <v>281</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="2" t="s">
         <v>516</v>
       </c>
       <c r="D67" t="s">
         <v>282</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E67" s="1">
         <v>1230</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="H67" s="6" t="s">
+      <c r="H67" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="I67" s="6" t="s">
+      <c r="I67" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="18.95" customHeight="1">
       <c r="A68" t="s">
         <v>286</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="2" t="s">
         <v>517</v>
       </c>
       <c r="D68" t="s">
         <v>287</v>
       </c>
-      <c r="E68" s="5">
+      <c r="E68" s="1">
         <v>1555</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="H68" s="6" t="s">
+      <c r="H68" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I68" s="6" t="s">
+      <c r="I68" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="18.95" customHeight="1">
       <c r="A69" t="s">
         <v>291</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="2" t="s">
         <v>518</v>
       </c>
       <c r="D69" t="s">
         <v>292</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="1">
         <v>1571</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="3" t="s">
         <v>293</v>
       </c>
       <c r="H69" t="s">
         <v>294</v>
       </c>
-      <c r="I69" s="6" t="s">
+      <c r="I69" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="18.95" customHeight="1">
       <c r="A70" t="s">
         <v>296</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="2" t="s">
         <v>519</v>
       </c>
       <c r="D70" t="s">
         <v>297</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E70" s="1">
         <v>1650</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="H70" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="I70" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="18.95" customHeight="1">
       <c r="A71" t="s">
         <v>301</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="2" t="s">
         <v>520</v>
       </c>
       <c r="D71" t="s">
         <v>297</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71" s="1">
         <v>1691</v>
       </c>
-      <c r="F71" s="7" t="s">
+      <c r="F71" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H71" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="I71" s="6" t="s">
+      <c r="I71" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="18.95" customHeight="1">
       <c r="A72" t="s">
         <v>305</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="2" t="s">
         <v>521</v>
       </c>
       <c r="D72" t="s">
         <v>297</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="1">
         <v>1215</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="H72" s="6" t="s">
+      <c r="H72" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I72" s="6" t="s">
+      <c r="I72" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="18.95" customHeight="1">
       <c r="A73" t="s">
         <v>309</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="2" t="s">
         <v>522</v>
       </c>
       <c r="D73" t="s">
         <v>297</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="1">
         <v>1657</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="H73" s="6" t="s">
+      <c r="H73" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="I73" s="6" t="s">
+      <c r="I73" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="18.95" customHeight="1">
       <c r="A74" t="s">
         <v>313</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="2" t="s">
         <v>523</v>
       </c>
       <c r="D74" t="s">
         <v>297</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="1">
         <v>1620</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="H74" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="I74" s="6" t="s">
+      <c r="I74" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="18.95" customHeight="1">
       <c r="A75" t="s">
         <v>317</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="2" t="s">
         <v>524</v>
       </c>
       <c r="D75" t="s">
         <v>297</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="1">
         <v>1665</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H75" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="I75" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="18.95" customHeight="1">
       <c r="A76" t="s">
         <v>321</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="2" t="s">
         <v>525</v>
       </c>
       <c r="D76" t="s">
         <v>297</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="1">
         <v>1695</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="H76" s="6" t="s">
+      <c r="H76" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="I76" s="6" t="s">
+      <c r="I76" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="18.95" customHeight="1">
       <c r="A77" t="s">
         <v>326</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="2" t="s">
         <v>526</v>
       </c>
       <c r="D77" t="s">
         <v>327</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="F77" s="7" t="s">
+      <c r="E77" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>328</v>
       </c>
       <c r="G77" t="s">
         <v>337</v>
       </c>
-      <c r="H77" s="6" t="s">
+      <c r="H77" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="I77" s="6" t="s">
+      <c r="I77" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="18.95" customHeight="1">
       <c r="A78" t="s">
         <v>331</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="1">
         <v>1690</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F78" s="3" t="s">
         <v>332</v>
       </c>
       <c r="G78" t="s">
         <v>333</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="H78" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="I78" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+    <row r="79" spans="1:9" ht="18.95" customHeight="1">
+      <c r="A79" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="11" t="s">
+      <c r="B79" s="3"/>
+      <c r="C79" s="7" t="s">
         <v>528</v>
       </c>
       <c r="D79" t="s">
         <v>327</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="1">
         <v>1870</v>
       </c>
-      <c r="F79" s="7" t="s">
+      <c r="F79" s="3" t="s">
         <v>335</v>
       </c>
       <c r="G79" t="s">
         <v>338</v>
       </c>
-      <c r="H79" s="6" t="s">
+      <c r="H79" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="I79" s="6" t="s">
+      <c r="I79" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="18.95" customHeight="1">
       <c r="A80" t="s">
         <v>340</v>
       </c>
       <c r="B80" t="s">
         <v>531</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="2" t="s">
         <v>529</v>
       </c>
       <c r="D80" t="s">
         <v>327</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="1">
         <v>1676</v>
       </c>
-      <c r="F80" s="7" t="s">
+      <c r="F80" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="H80" s="6" t="s">
+      <c r="H80" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I80" s="6" t="s">
+      <c r="I80" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="18.95" customHeight="1">
       <c r="A81" t="s">
         <v>342</v>
       </c>
       <c r="B81" t="s">
         <v>532</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="2" t="s">
         <v>530</v>
       </c>
       <c r="D81" t="s">
         <v>327</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="1">
         <v>1677</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="H81" s="6" t="s">
+      <c r="H81" s="2" t="s">
         <v>344</v>
       </c>
       <c r="I81" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="18.95" customHeight="1">
       <c r="A82" t="s">
         <v>355</v>
       </c>
       <c r="B82" t="s">
         <v>356</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D82" t="s">
         <v>358</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82" s="1">
         <v>323</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F82" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="H82" s="6" t="s">
+      <c r="H82" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="I82" s="6" t="s">
+      <c r="I82" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="18.95" customHeight="1">
       <c r="A83" t="s">
         <v>362</v>
       </c>
       <c r="B83" t="s">
         <v>363</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="2" t="s">
         <v>364</v>
       </c>
       <c r="D83" t="s">
         <v>365</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="1">
         <v>1590</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="F83" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="H83" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="I83" s="6" t="s">
+      <c r="I83" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="18.95" customHeight="1">
       <c r="A84" t="s">
         <v>369</v>
       </c>
       <c r="B84" t="s">
         <v>370</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="2" t="s">
         <v>371</v>
       </c>
       <c r="D84" t="s">
         <v>372</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="1">
         <v>960</v>
       </c>
-      <c r="F84" s="7" t="s">
+      <c r="F84" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="H84" s="6" t="s">
+      <c r="H84" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="I84" s="6" t="s">
+      <c r="I84" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="18.95" customHeight="1">
       <c r="A85" t="s">
         <v>376</v>
       </c>
       <c r="B85" t="s">
         <v>377</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="2" t="s">
         <v>378</v>
       </c>
       <c r="D85" t="s">
         <v>379</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85" s="1">
         <v>1050</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F85" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="H85" s="6" t="s">
+      <c r="H85" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="I85" s="6" t="s">
+      <c r="I85" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="18.95" customHeight="1">
       <c r="A86" t="s">
         <v>383</v>
       </c>
       <c r="B86" t="s">
         <v>384</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="2" t="s">
         <v>385</v>
       </c>
       <c r="D86" t="s">
         <v>386</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="1">
         <v>1280</v>
       </c>
-      <c r="F86" s="7" t="s">
+      <c r="F86" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="H86" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="18.95" customHeight="1">
       <c r="A87" t="s">
         <v>389</v>
       </c>
       <c r="B87" t="s">
         <v>390</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D87" t="s">
         <v>392</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E87" s="1">
         <v>1259</v>
       </c>
-      <c r="F87" s="7" t="s">
+      <c r="F87" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="H87" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="I87" s="6" t="s">
+      <c r="I87" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="18.95" customHeight="1">
       <c r="A88" t="s">
         <v>396</v>
       </c>
       <c r="B88" t="s">
         <v>397</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="2" t="s">
         <v>398</v>
       </c>
       <c r="D88" t="s">
         <v>392</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="1">
         <v>537</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="F88" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="H88" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="I88" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="18.95" customHeight="1">
       <c r="A89" t="s">
         <v>221</v>
       </c>
       <c r="B89" t="s">
         <v>402</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="2" t="s">
         <v>403</v>
       </c>
       <c r="D89" t="s">
         <v>404</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="F89" s="7" t="s">
+      <c r="F89" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="H89" s="6" t="s">
+      <c r="H89" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="I89" s="6" t="s">
+      <c r="I89" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="18.95" customHeight="1">
       <c r="A90" t="s">
         <v>408</v>
       </c>
       <c r="B90" t="s">
         <v>409</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="2" t="s">
         <v>410</v>
       </c>
       <c r="D90" t="s">
         <v>411</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F90" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="H90" s="6" t="s">
+      <c r="H90" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="I90" s="6" t="s">
+      <c r="I90" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="18.95" customHeight="1">
       <c r="A91" t="s">
         <v>415</v>
       </c>
       <c r="B91" t="s">
         <v>416</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="2" t="s">
         <v>417</v>
       </c>
       <c r="D91" t="s">
         <v>418</v>
       </c>
-      <c r="E91" s="5">
+      <c r="E91" s="1">
         <v>1230</v>
       </c>
-      <c r="F91" s="7" t="s">
+      <c r="F91" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="H91" s="6" t="s">
+      <c r="H91" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I91" s="6" t="s">
+      <c r="I91" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="18.95" customHeight="1">
       <c r="A92" t="s">
         <v>422</v>
       </c>
       <c r="B92" t="s">
         <v>423</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D92" t="s">
         <v>425</v>
       </c>
-      <c r="E92" s="5">
+      <c r="E92" s="1">
         <v>1306</v>
       </c>
-      <c r="F92" s="7" t="s">
+      <c r="F92" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="H92" s="6" t="s">
+      <c r="H92" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="I92" s="6" t="s">
+      <c r="I92" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="18.95" customHeight="1">
       <c r="A93" t="s">
         <v>429</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C93" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D93" t="s">
         <v>431</v>
       </c>
-      <c r="E93" s="5">
+      <c r="E93" s="1">
         <v>1320</v>
       </c>
-      <c r="F93" s="7" t="s">
+      <c r="F93" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="H93" s="6" t="s">
+      <c r="H93" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="18.95" customHeight="1">
       <c r="A94" t="s">
         <v>434</v>
       </c>
       <c r="B94" t="s">
         <v>435</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="2" t="s">
         <v>436</v>
       </c>
       <c r="D94" t="s">
         <v>437</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E94" s="1">
         <v>1295</v>
       </c>
-      <c r="F94" s="7" t="s">
+      <c r="F94" s="3" t="s">
         <v>438</v>
       </c>
       <c r="H94" t="s">
         <v>439</v>
       </c>
-      <c r="I94" s="6" t="s">
+      <c r="I94" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="18.95" customHeight="1">
       <c r="A95" t="s">
         <v>408</v>
       </c>
       <c r="B95" t="s">
         <v>441</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C95" s="2" t="s">
         <v>442</v>
       </c>
       <c r="D95" t="s">
         <v>443</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="1">
         <v>1380</v>
       </c>
-      <c r="F95" s="7" t="s">
+      <c r="F95" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="H95" s="6" t="s">
+      <c r="H95" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="I95" s="6" t="s">
+      <c r="I95" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="18.95" customHeight="1">
       <c r="A96" t="s">
         <v>447</v>
       </c>
       <c r="B96" t="s">
         <v>448</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C96" s="2" t="s">
         <v>449</v>
       </c>
       <c r="D96" t="s">
         <v>450</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="1">
         <v>2004</v>
       </c>
-      <c r="F96" s="7" t="s">
+      <c r="F96" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="H96" s="6" t="s">
+      <c r="H96" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="I96" s="6" t="s">
+      <c r="I96" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>133</v>
       </c>
       <c r="B97" t="s">
         <v>538</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="2" t="s">
         <v>539</v>
       </c>
       <c r="D97" t="s">
         <v>540</v>
       </c>
-      <c r="E97" s="5">
+      <c r="E97" s="1">
         <v>1994</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F97" s="1" t="s">
         <v>541</v>
       </c>
       <c r="G97" t="s">
         <v>543</v>
       </c>
-      <c r="H97" s="6" t="s">
+      <c r="H97" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="I97" s="6" t="s">
+      <c r="I97" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>544</v>
       </c>
       <c r="B98" t="s">
         <v>545</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="2" t="s">
         <v>546</v>
       </c>
       <c r="D98" t="s">
         <v>540</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98" s="1">
         <v>1472</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F98" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="H98" s="6" t="s">
+      <c r="H98" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="I98" s="6" t="s">
+      <c r="I98" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>551</v>
       </c>
@@ -5121,99 +5457,503 @@
       <c r="D99" t="s">
         <v>540</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99" s="1">
         <v>1555</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="I99" s="6" t="s">
+      <c r="H99" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="I99" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>555</v>
       </c>
       <c r="B100" t="s">
         <v>556</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="2" t="s">
         <v>557</v>
       </c>
       <c r="D100" t="s">
         <v>540</v>
       </c>
-      <c r="E100" s="5">
+      <c r="E100" s="1">
         <v>1845</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F100" s="1" t="s">
         <v>560</v>
       </c>
       <c r="G100" t="s">
         <v>558</v>
       </c>
-      <c r="H100" s="6" t="s">
+      <c r="H100" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="I100" s="6" t="s">
+      <c r="I100" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>561</v>
       </c>
       <c r="B101" t="s">
         <v>562</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C101" s="2" t="s">
         <v>563</v>
       </c>
       <c r="D101" t="s">
         <v>540</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101" s="1">
         <v>1591</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F101" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="H101" s="6" t="s">
+      <c r="H101" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="I101" s="6" t="s">
+      <c r="I101" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>566</v>
       </c>
       <c r="B102" t="s">
         <v>567</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="2" t="s">
         <v>568</v>
       </c>
       <c r="D102" t="s">
         <v>540</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E102" s="1">
         <v>1524</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="H102" s="6" t="s">
+      <c r="H102" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="I102" s="6" t="s">
+      <c r="I102" s="2" t="s">
         <v>549</v>
       </c>
     </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>576</v>
+      </c>
+      <c r="B103" t="s">
+        <v>577</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D103" t="s">
+        <v>579</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1051</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="G103" t="s">
+        <v>581</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>585</v>
+      </c>
+      <c r="B104" t="s">
+        <v>586</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D104" t="s">
+        <v>587</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1655</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="G104" t="s">
+        <v>591</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>593</v>
+      </c>
+      <c r="B105" t="s">
+        <v>596</v>
+      </c>
+      <c r="C105" t="s">
+        <v>595</v>
+      </c>
+      <c r="D105" t="s">
+        <v>594</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1995</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="G105" t="s">
+        <v>599</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>601</v>
+      </c>
+      <c r="B106" t="s">
+        <v>602</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D106" t="s">
+        <v>603</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1997</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="G106" t="s">
+        <v>607</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>609</v>
+      </c>
+      <c r="B107" t="s">
+        <v>610</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D107" t="s">
+        <v>611</v>
+      </c>
+      <c r="E107" s="1">
+        <v>1679</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>616</v>
+      </c>
+      <c r="B108" t="s">
+        <v>618</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D108" t="s">
+        <v>617</v>
+      </c>
+      <c r="E108" s="1">
+        <v>1633</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>623</v>
+      </c>
+      <c r="B109" t="s">
+        <v>625</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D109" t="s">
+        <v>680</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1994</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="G109" t="s">
+        <v>628</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>630</v>
+      </c>
+      <c r="B110" t="s">
+        <v>633</v>
+      </c>
+      <c r="C110" t="s">
+        <v>632</v>
+      </c>
+      <c r="D110" t="s">
+        <v>631</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1861</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>636</v>
+      </c>
+      <c r="B111" t="s">
+        <v>639</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D111" t="s">
+        <v>637</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1830</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>644</v>
+      </c>
+      <c r="B112" t="s">
+        <v>646</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="D112" t="s">
+        <v>645</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1180</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>555</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="D113" t="s">
+        <v>650</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1761</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>656</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D114" t="s">
+        <v>658</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>664</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="D115" t="s">
+        <v>681</v>
+      </c>
+      <c r="E115" s="1">
+        <v>2004</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>669</v>
+      </c>
+      <c r="B116" t="s">
+        <v>670</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="D116" t="s">
+        <v>671</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1825</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>675</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D117" t="s">
+        <v>675</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1195</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
     <hyperlink ref="I2" r:id="rId2"/>
@@ -5506,26 +6246,73 @@
     <hyperlink ref="C102" r:id="rId289"/>
     <hyperlink ref="H102" r:id="rId290"/>
     <hyperlink ref="I102" r:id="rId291"/>
+    <hyperlink ref="C103" r:id="rId292"/>
+    <hyperlink ref="H99" r:id="rId293"/>
+    <hyperlink ref="H103" r:id="rId294"/>
+    <hyperlink ref="I103" r:id="rId295"/>
+    <hyperlink ref="C104" r:id="rId296"/>
+    <hyperlink ref="I104" r:id="rId297"/>
+    <hyperlink ref="H104" r:id="rId298"/>
+    <hyperlink ref="I105" r:id="rId299"/>
+    <hyperlink ref="H105" r:id="rId300"/>
+    <hyperlink ref="C106" r:id="rId301"/>
+    <hyperlink ref="I106" r:id="rId302"/>
+    <hyperlink ref="H106" r:id="rId303"/>
+    <hyperlink ref="C107" r:id="rId304"/>
+    <hyperlink ref="I107" r:id="rId305"/>
+    <hyperlink ref="H107" r:id="rId306"/>
+    <hyperlink ref="C108" r:id="rId307"/>
+    <hyperlink ref="I108" r:id="rId308"/>
+    <hyperlink ref="H108" r:id="rId309"/>
+    <hyperlink ref="C109" r:id="rId310"/>
+    <hyperlink ref="I109" r:id="rId311"/>
+    <hyperlink ref="H109" r:id="rId312"/>
+    <hyperlink ref="H110" r:id="rId313"/>
+    <hyperlink ref="C111" r:id="rId314"/>
+    <hyperlink ref="I111" r:id="rId315"/>
+    <hyperlink ref="H111" r:id="rId316"/>
+    <hyperlink ref="I112" r:id="rId317"/>
+    <hyperlink ref="C112" r:id="rId318"/>
+    <hyperlink ref="H112" r:id="rId319"/>
+    <hyperlink ref="C113" r:id="rId320"/>
+    <hyperlink ref="B113" r:id="rId321" location="/maplink/0" display="https://ru.wikipedia.org/wiki/%D0%91%D0%BE%D0%B3%D0%BE%D1%8F%D0%B2%D0%BB%D0%B5%D0%BD%D1%81%D0%BA%D0%B8%D0%B9_%D1%81%D0%BE%D0%B1%D0%BE%D1%80_(%D0%9F%D0%BE%D0%BB%D0%BE%D1%86%D0%BA) - /maplink/0"/>
+    <hyperlink ref="H113" r:id="rId322"/>
+    <hyperlink ref="I113" r:id="rId323"/>
+    <hyperlink ref="B114" r:id="rId324" location="/maplink/0" display="https://ru.wikipedia.org/wiki/%D0%A1%D0%B2%D0%B5%D1%82%D0%B8%D1%86%D1%85%D0%BE%D0%B2%D0%B5%D0%BB%D0%B8 - /maplink/0"/>
+    <hyperlink ref="C114" r:id="rId325"/>
+    <hyperlink ref="I114" r:id="rId326"/>
+    <hyperlink ref="H114" r:id="rId327"/>
+    <hyperlink ref="B115" r:id="rId328" location="/maplink/0" display="https://ru.wikipedia.org/wiki/%D0%A6%D0%BC%D0%B8%D0%BD%D0%B4%D0%B0_%D0%A1%D0%B0%D0%BC%D0%B5%D0%B1%D0%B0 - /maplink/0"/>
+    <hyperlink ref="C115" r:id="rId329"/>
+    <hyperlink ref="I115" r:id="rId330"/>
+    <hyperlink ref="H115" r:id="rId331"/>
+    <hyperlink ref="C116" r:id="rId332"/>
+    <hyperlink ref="H116" r:id="rId333"/>
+    <hyperlink ref="I116" r:id="rId334"/>
+    <hyperlink ref="B117" r:id="rId335" location="/maplink/0" display="https://ru.wikipedia.org/wiki/%D0%A2%D0%B8%D0%BC%D0%BE%D1%82%D0%B5%D1%81%D1%83%D0%B1%D0%B0%D0%BD%D0%B8_(%D1%85%D1%80%D0%B0%D0%BC) - /maplink/0"/>
+    <hyperlink ref="C117" r:id="rId336"/>
+    <hyperlink ref="I117" r:id="rId337"/>
+    <hyperlink ref="H117" r:id="rId338"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId339"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5548,36 +6335,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="5" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="6" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="7" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="8" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="9" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="10" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="11" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="12" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="13" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="14" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="15" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="16" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="17" ht="18.95" customHeight="1"/>
+    <row r="18" ht="18.95" customHeight="1"/>
+    <row r="19" ht="18.95" customHeight="1"/>
+    <row r="20" ht="18.95" customHeight="1"/>
+    <row r="21" ht="18.95" customHeight="1"/>
+    <row r="22" ht="18.95" customHeight="1"/>
+    <row r="23" ht="18.95" customHeight="1"/>
+    <row r="24" ht="18.95" customHeight="1"/>
+    <row r="25" ht="18.95" customHeight="1"/>
+    <row r="26" ht="18.95" customHeight="1"/>
+    <row r="27" ht="18.95" customHeight="1"/>
+    <row r="28" ht="18.95" customHeight="1"/>
+    <row r="29" ht="18.95" customHeight="1"/>
+    <row r="30" ht="18.95" customHeight="1"/>
+    <row r="31" ht="18.95" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -5585,19 +6372,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5620,16 +6407,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="5" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="6" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="7" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="8" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="9" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="10" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="11" spans="1:7" ht="18.95" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -5637,20 +6424,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5673,14 +6460,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="5" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="6" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="7" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="8" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="9" spans="1:7" ht="18.95" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add image for temples and personsreligions add quote to about page
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/храмы.xlsx
+++ b/loadDatabase/religion/храмы.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$J$117</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1590,9 +1593,6 @@
     <t>39°37′30″ с. ш. 19°55′22″ в. д.</t>
   </si>
   <si>
-    <t>https://azbyka.ru/palomnik/images/thumb/a/a0/Собор_святителя_Спиридона_%28Керкира%29.jpg/772px-Собор_святителя_Спиридона_%28Керкира%29.jpg</t>
-  </si>
-  <si>
     <t>г. Керкира, о-в Корфу, Греция</t>
   </si>
   <si>
@@ -1748,9 +1748,6 @@
     <t>42°16′15″ с. ш. 22°40′37″ в. д.</t>
   </si>
   <si>
-    <t>https://azbyka.ru/palomnik/images/thumb/a/a7/Церковь_святого_Георгия_Победоносца_%28Кюстендил%293.jpg/600px-Церковь_святого_Георгия_Победоносца_%28Кюстендил%293.jpg</t>
-  </si>
-  <si>
     <t>г. Кюстендил, Болгария</t>
   </si>
   <si>
@@ -1792,9 +1789,6 @@
   </si>
   <si>
     <t>43°05′04″ с. ш. 25°39′00″ в. д.</t>
-  </si>
-  <si>
-    <t>https://azbyka.ru/palomnik/images/0/09/Церковь_Сорока_Великомучеников_%28Велико-Тырново%294.jpg</t>
   </si>
   <si>
     <t>г. Велико-Тырново, Болгария</t>
@@ -2002,9 +1996,6 @@
     <t>https://avatars.mds.yandex.net/get-altay/904281/2a00000162870a8f6509c9e06d0c389cbcaa/XXL</t>
   </si>
   <si>
-    <t>http://gidavia.com/wp-content/uploads/2020/01/chto-posmotret-v-tolyatti-cerkvi.jpg</t>
-  </si>
-  <si>
     <t>http://temples.ru/private/f000264/264_0133738b.jpg</t>
   </si>
   <si>
@@ -2014,9 +2005,6 @@
     <t>https://avatars.mds.yandex.net/get-altay/367090/2a00000162874eb3d58541fd1b2b27855b7e/XXL</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/f/f3/Церковь_Казанской_иконы_Божьей_Матери_%28Верхнее_Санчелеево%29.jpg</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/5/50/Tashelka_7515.jpg</t>
   </si>
   <si>
@@ -2150,9 +2138,6 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/6/64/Church_of_the_Saviour_on_the_Town_in_Yaroslavl_01.jpg/1280px-Church_of_the_Saviour_on_the_Town_in_Yaroslavl_01.jpg</t>
-  </si>
-  <si>
-    <t>http://gidavia.com/wp-content/uploads/2018/11/10-%D0%A1%D0%BF%D0%B0%D1%81%D0%BE-%D0%9F%D1%80%D0%B5%D0%BE%D0%B1%D1%80%D0%B0%D0%B6%D0%B5%D0%BD%D1%81%D0%BA%D0%B8%D0%B9-%D1%81%D0%BE%D0%B1%D0%BE%D1%80.jpg</t>
   </si>
   <si>
     <t>http://temples.ru/private/f000204/204_0076600b.jpg</t>
@@ -2619,6 +2604,24 @@
   </si>
   <si>
     <t>Тбилиси</t>
+  </si>
+  <si>
+    <t>https://azbyka.ru/palomnik/images/0/09/Церковь_Сорока_Великомучеников_(Велико-Тырново)4.jpg</t>
+  </si>
+  <si>
+    <t>https://azbyka.ru/palomnik/images/thumb/a/a7/Церковь_святого_Георгия_Победоносца_(Кюстендил)3.jpg/600px-Церковь_святого_Георгия_Победоносца_(Кюстендил)3.jpg</t>
+  </si>
+  <si>
+    <t>https://sobory.ru/pic/30500/30538bb.jpg</t>
+  </si>
+  <si>
+    <t>https://www.corfugid.ru/images/12096009_10206504350782578_2883688206643119801_n.jpg</t>
+  </si>
+  <si>
+    <t>https://photos.wikimapia.org/p/00/05/84/43/87_big.jpg</t>
+  </si>
+  <si>
+    <t>https://choirvera.ru/wp-content/uploads/2019/04/Sobor_spasa_preobrazheniya_v_tambove__rossiya__gorod_tambov_1.jpg</t>
   </si>
 </sst>
 </file>
@@ -3036,7 +3039,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -3079,7 +3082,7 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>12</v>
@@ -3105,7 +3108,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>325</v>
@@ -3131,7 +3134,7 @@
         <v>347</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -3157,7 +3160,7 @@
         <v>350</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -3180,10 +3183,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -3206,10 +3209,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
@@ -3226,7 +3229,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -3252,10 +3255,10 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -3275,7 +3278,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -3289,7 +3292,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>32</v>
@@ -3312,7 +3315,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>32</v>
@@ -3335,13 +3338,13 @@
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>41</v>
@@ -3362,7 +3365,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
@@ -3385,7 +3388,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>32</v>
@@ -3408,7 +3411,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>32</v>
@@ -3431,7 +3434,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>32</v>
@@ -3454,7 +3457,7 @@
         <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>32</v>
@@ -3477,7 +3480,7 @@
         <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>32</v>
@@ -3500,7 +3503,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>32</v>
@@ -3523,7 +3526,7 @@
         <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>32</v>
@@ -3546,7 +3549,7 @@
         <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>32</v>
@@ -3570,7 +3573,7 @@
         <v>81</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>82</v>
@@ -3593,7 +3596,7 @@
         <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>87</v>
@@ -3616,7 +3619,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>92</v>
@@ -3639,7 +3642,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>97</v>
@@ -3662,7 +3665,7 @@
         <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>476</v>
+        <v>680</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>102</v>
@@ -3685,7 +3688,7 @@
         <v>105</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>102</v>
@@ -3708,7 +3711,7 @@
         <v>110</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>111</v>
@@ -3728,7 +3731,7 @@
         <v>114</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>480</v>
+        <v>678</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>115</v>
@@ -3751,7 +3754,7 @@
         <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>119</v>
@@ -3774,7 +3777,7 @@
         <v>123</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>124</v>
@@ -3797,7 +3800,7 @@
         <v>128</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>129</v>
@@ -3820,7 +3823,7 @@
         <v>133</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>97</v>
@@ -3847,7 +3850,7 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="6" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>139</v>
@@ -3872,7 +3875,7 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="6" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>139</v>
@@ -3899,13 +3902,13 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="6" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>149</v>
@@ -3924,7 +3927,7 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="6" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>139</v>
@@ -3949,7 +3952,7 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="6" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>139</v>
@@ -3974,7 +3977,7 @@
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="6" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>139</v>
@@ -3999,7 +4002,7 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="6" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>139</v>
@@ -4024,7 +4027,7 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="6" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>139</v>
@@ -4049,7 +4052,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="6" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>139</v>
@@ -4074,7 +4077,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="6" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>139</v>
@@ -4099,7 +4102,7 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>139</v>
@@ -4124,7 +4127,7 @@
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="6" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>139</v>
@@ -4149,7 +4152,7 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="6" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>139</v>
@@ -4174,7 +4177,7 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="6" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>139</v>
@@ -4199,7 +4202,7 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="6" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>139</v>
@@ -4224,7 +4227,7 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="6" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>139</v>
@@ -4249,7 +4252,7 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="6" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>205</v>
@@ -4276,7 +4279,7 @@
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="6" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>211</v>
@@ -4301,7 +4304,7 @@
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="6" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>216</v>
@@ -4326,7 +4329,7 @@
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="6" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>139</v>
@@ -4351,7 +4354,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>139</v>
@@ -4376,7 +4379,7 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="6" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>139</v>
@@ -4401,7 +4404,7 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="6" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>139</v>
@@ -4426,7 +4429,7 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="6" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>139</v>
@@ -4451,7 +4454,7 @@
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="6" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>139</v>
@@ -4478,7 +4481,7 @@
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="6" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>245</v>
@@ -4505,7 +4508,7 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="6" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>251</v>
@@ -4530,7 +4533,7 @@
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="6" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>256</v>
@@ -4554,7 +4557,7 @@
         <v>260</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D63" t="s">
         <v>261</v>
@@ -4580,7 +4583,7 @@
         <v>266</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D64" t="s">
         <v>261</v>
@@ -4603,7 +4606,7 @@
         <v>270</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D65" t="s">
         <v>271</v>
@@ -4626,7 +4629,7 @@
         <v>275</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D66" t="s">
         <v>276</v>
@@ -4652,7 +4655,7 @@
         <v>281</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="D67" t="s">
         <v>282</v>
@@ -4675,7 +4678,7 @@
         <v>286</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D68" t="s">
         <v>287</v>
@@ -4698,7 +4701,7 @@
         <v>291</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D69" t="s">
         <v>292</v>
@@ -4721,7 +4724,7 @@
         <v>296</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D70" t="s">
         <v>297</v>
@@ -4744,7 +4747,7 @@
         <v>301</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="D71" t="s">
         <v>297</v>
@@ -4767,7 +4770,7 @@
         <v>305</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D72" t="s">
         <v>297</v>
@@ -4790,7 +4793,7 @@
         <v>309</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D73" t="s">
         <v>297</v>
@@ -4813,7 +4816,7 @@
         <v>313</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D74" t="s">
         <v>297</v>
@@ -4836,7 +4839,7 @@
         <v>317</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="D75" t="s">
         <v>297</v>
@@ -4859,7 +4862,7 @@
         <v>321</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D76" t="s">
         <v>297</v>
@@ -4882,13 +4885,13 @@
         <v>326</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>526</v>
+        <v>681</v>
       </c>
       <c r="D77" t="s">
         <v>327</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>328</v>
@@ -4908,7 +4911,7 @@
         <v>331</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>327</v>
@@ -4935,7 +4938,7 @@
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="7" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="D79" t="s">
         <v>327</v>
@@ -4961,10 +4964,10 @@
         <v>340</v>
       </c>
       <c r="B80" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="D80" t="s">
         <v>327</v>
@@ -4987,10 +4990,10 @@
         <v>342</v>
       </c>
       <c r="B81" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="D81" t="s">
         <v>327</v>
@@ -5042,149 +5045,149 @@
         <v>363</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="D83" t="s">
         <v>364</v>
-      </c>
-      <c r="D83" t="s">
-        <v>365</v>
       </c>
       <c r="E83" s="1">
         <v>1590</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="18.95" customHeight="1">
       <c r="A84" t="s">
+        <v>368</v>
+      </c>
+      <c r="B84" t="s">
         <v>369</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" t="s">
         <v>371</v>
-      </c>
-      <c r="D84" t="s">
-        <v>372</v>
       </c>
       <c r="E84" s="1">
         <v>960</v>
       </c>
       <c r="F84" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="18.95" customHeight="1">
       <c r="A85" t="s">
+        <v>375</v>
+      </c>
+      <c r="B85" t="s">
         <v>376</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" t="s">
         <v>378</v>
-      </c>
-      <c r="D85" t="s">
-        <v>379</v>
       </c>
       <c r="E85" s="1">
         <v>1050</v>
       </c>
       <c r="F85" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18.95" customHeight="1">
       <c r="A86" t="s">
+        <v>382</v>
+      </c>
+      <c r="B86" t="s">
         <v>383</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" t="s">
         <v>385</v>
-      </c>
-      <c r="D86" t="s">
-        <v>386</v>
       </c>
       <c r="E86" s="1">
         <v>1280</v>
       </c>
       <c r="F86" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="18.95" customHeight="1">
       <c r="A87" t="s">
+        <v>388</v>
+      </c>
+      <c r="B87" t="s">
         <v>389</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" t="s">
         <v>391</v>
-      </c>
-      <c r="D87" t="s">
-        <v>392</v>
       </c>
       <c r="E87" s="1">
         <v>1259</v>
       </c>
       <c r="F87" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="I87" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="18.95" customHeight="1">
       <c r="A88" t="s">
+        <v>395</v>
+      </c>
+      <c r="B88" t="s">
         <v>396</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="D88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E88" s="1">
         <v>537</v>
       </c>
       <c r="F88" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="I88" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="18.95" customHeight="1">
@@ -5192,201 +5195,201 @@
         <v>221</v>
       </c>
       <c r="B89" t="s">
+        <v>401</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D89" t="s">
         <v>402</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="E89" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="D89" t="s">
+      <c r="H89" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="F89" s="3" t="s">
+      <c r="I89" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="18.95" customHeight="1">
       <c r="A90" t="s">
+        <v>406</v>
+      </c>
+      <c r="B90" t="s">
+        <v>407</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>409</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="E90" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="D90" t="s">
+      <c r="H90" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="F90" s="3" t="s">
+      <c r="I90" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="18.95" customHeight="1">
       <c r="A91" t="s">
+        <v>413</v>
+      </c>
+      <c r="B91" t="s">
+        <v>414</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="D91" t="s">
         <v>415</v>
-      </c>
-      <c r="B91" t="s">
-        <v>416</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D91" t="s">
-        <v>418</v>
       </c>
       <c r="E91" s="1">
         <v>1230</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="18.95" customHeight="1">
       <c r="A92" t="s">
+        <v>419</v>
+      </c>
+      <c r="B92" t="s">
+        <v>420</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D92" t="s">
         <v>422</v>
-      </c>
-      <c r="B92" t="s">
-        <v>423</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D92" t="s">
-        <v>425</v>
       </c>
       <c r="E92" s="1">
         <v>1306</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="18.95" customHeight="1">
       <c r="A93" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D93" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E93" s="1">
         <v>1320</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18.95" customHeight="1">
       <c r="A94" t="s">
+        <v>431</v>
+      </c>
+      <c r="B94" t="s">
+        <v>432</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D94" t="s">
         <v>434</v>
-      </c>
-      <c r="B94" t="s">
-        <v>435</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="D94" t="s">
-        <v>437</v>
       </c>
       <c r="E94" s="1">
         <v>1295</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H94" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="18.95" customHeight="1">
       <c r="A95" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B95" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D95" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E95" s="1">
         <v>1380</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="18.95" customHeight="1">
       <c r="A96" t="s">
+        <v>444</v>
+      </c>
+      <c r="B96" t="s">
+        <v>445</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D96" t="s">
         <v>447</v>
-      </c>
-      <c r="B96" t="s">
-        <v>448</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D96" t="s">
-        <v>450</v>
       </c>
       <c r="E96" s="1">
         <v>2004</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -5394,566 +5397,567 @@
         <v>133</v>
       </c>
       <c r="B97" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D97" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E97" s="1">
         <v>1994</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="G97" t="s">
+        <v>537</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="I97" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="B98" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D98" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E98" s="1">
         <v>1472</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B99" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="C99" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="D99" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E99" s="1">
         <v>1555</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B100" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D100" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E100" s="1">
         <v>1845</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="G100" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="B101" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="D101" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E101" s="1">
         <v>1591</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B102" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D102" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E102" s="1">
         <v>1524</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B103" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="D103" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="E103" s="1">
         <v>1051</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="G103" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B104" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="D104" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="E104" s="1">
         <v>1655</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="G104" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B105" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C105" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="D105" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="E105" s="1">
         <v>1995</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="G105" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B106" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="D106" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="E106" s="1">
         <v>1997</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="G106" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B107" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="D107" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="E107" s="1">
         <v>1679</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B108" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="D108" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="E108" s="1">
         <v>1633</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B109" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="D109" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="E109" s="1">
         <v>1994</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="G109" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B110" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C110" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="D110" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E110" s="1">
         <v>1861</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B111" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="D111" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="E111" s="1">
         <v>1830</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B112" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="D112" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="E112" s="1">
         <v>1180</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="D113" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="E113" s="1">
         <v>1761</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
+        <v>650</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D114" t="s">
+        <v>652</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="H114" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="D114" t="s">
-        <v>658</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="I114" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="D115" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="E115" s="1">
         <v>2004</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B116" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D116" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="E116" s="1">
         <v>1825</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="D117" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="E117" s="1">
         <v>1195</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J117"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
     <hyperlink ref="I2" r:id="rId2"/>

</xml_diff>

<commit_message>
Add new images for temples
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/храмы.xlsx
+++ b/loadDatabase/religion/храмы.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="746">
   <si>
     <t>название</t>
   </si>
@@ -2700,6 +2700,120 @@
   </si>
   <si>
     <t>01.11.2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/fLFz/JCkkJmGrq  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/UVjT/mUWFVeZK9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/xqu4/1oYTqbzPq </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/756N/f7Dzx6XpU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/rfr3/pJhqLHmhb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/WoFC/38HbhVjeA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/swjt/z5bVYica6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/5oiH/w5o281EsT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/noVg/zkXSPHwzn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/ZeFd/UdyKufFX6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/iTtn/XraeBj5BL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/hVwo/GMmWjKyvp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/dmtU/FLuEZmzFD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/Eon3/eLJaD8EF7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/oMHz/JqMeounYV </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cloud.mail.ru/public/KD7j/k4kCWWd6S </t>
+  </si>
+  <si>
+    <t>Троице-Серигиева Лавра</t>
+  </si>
+  <si>
+    <t>56°18′37″ с. ш. 38°07′46″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/8/8a/%D0%A1%D0%B5%D1%80%D0%B3%D0%B8%D0%B5%D0%B2_%D0%9F%D0%BE%D1%81%D0%B0%D0%B4._%D0%A2%D1%80%D0%BE%D0%B8%D1%86%D0%B5-%D0%A1%D0%B5%D1%80%D0%B3%D0%B8%D0%B5%D0%B2%D0%B0_%D0%BB%D0%B0%D0%B2%D1%80%D0%B0._1.jpg </t>
+  </si>
+  <si>
+    <t>Сериев Посад</t>
+  </si>
+  <si>
+    <t>Тро́ице-Се́ргиева ла́вра (в церковной литературе обычно Свя́то-Тро́ицкая Сергиева лавра) — крупнейший мужской монастырь Русской православной церкви с многовековой историей. Расположен в центре города Сергиева Посада Московской области, на реке Кончуре́. Имеет статус ставропигиального. Крупнейший центр образовательной и издательской деятельности Русской православной церкви. Место нахождения Московской духовной академии. В Свято-Троицком соборе лавры находятся мощи основателя монастыря, преподобного Сергия Радонежского.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Троице-Сергиева_лавра </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mepar.ru </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn21.img.ria.ru/images/156093/74/1560937403_285:0:2422:1202_600x0_80_0_0_76bfe47eb524426336884057a3e2700d.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdnimg.rg.ru/img/content/194/20/87/TASS_22911370_d_850.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn25.img.ria.ru/images/153218/34/1532183407_0:255:2733:1792_600x0_80_0_0_1cad8e0076ef6ddd6cac86048d924ef5.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img04.rl0.ru/afisha/e730x-i/daily.afisha.ru/uploads/images/4/e7/4e76e5cc5a9503d1ba5ce0b02406bd7e.jpg </t>
+  </si>
+  <si>
+    <t>Раваница</t>
+  </si>
+  <si>
+    <t>43°58′22″ с. ш. 21°29′48″ в. д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/0/0c/Monastery_Ravanica.JPG/1280px-Monastery_Ravanica.JPG </t>
+  </si>
+  <si>
+    <t>Сенье</t>
+  </si>
+  <si>
+    <t>Монастырь Раваница был возведён в 1375—1377 годах на средства князя Лазаря Хребеляновича, а в 1380-е годы главный храм был расписан. В 1389 году погибший в битве на Косовом поле Лазарь был похоронен в монастыре, позднее там же были погребены его вдова Милица и сыновья Стефан и Вук. В последующие годы монастырь неоднократно подвергался турецким нападениям, в 1690 году был оставлен братией, которые обосновались в заброшенном монастыре Врдник на Фрушке-горе, куда перенесли мощи праведного сербского князя.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Раваница_(монастырь)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sabornost.org/global/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://excursio.com/upload/excursions_photo/213388/92194_p_681x405_9b1f459309c8906e80c54c5ad8077b75.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.serbianprivatetours.com/wp-content/uploads/2016/05/monastery-manasija-tour-5.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sobory.ru/pic/35650/35675_20180510_211531.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://otdihvserbii.ru/wp-content/uploads/2014/11/Manastir_Ravanica_Vrdnik_3-1.jpg </t>
   </si>
 </sst>
 </file>
@@ -3121,8 +3235,8 @@
   <dimension ref="A1:N435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,6 +3515,18 @@
       <c r="I9" s="2" t="s">
         <v>316</v>
       </c>
+      <c r="J9" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -3539,6 +3665,18 @@
       <c r="I14" t="s">
         <v>316</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3926,10 +4064,18 @@
       <c r="I29" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
+      <c r="J29" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>711</v>
+      </c>
       <c r="N29" s="14"/>
     </row>
     <row r="30" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3956,6 +4102,18 @@
       </c>
       <c r="I30" s="2" t="s">
         <v>316</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5991,7 +6149,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>403</v>
       </c>
@@ -6011,7 +6169,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>392</v>
       </c>
@@ -6037,7 +6195,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -6057,7 +6215,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>631</v>
       </c>
@@ -6083,18 +6241,95 @@
         <v>628</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>724</v>
+      </c>
+      <c r="B117" t="s">
+        <v>725</v>
+      </c>
+      <c r="C117" t="s">
+        <v>726</v>
+      </c>
+      <c r="D117" t="s">
+        <v>727</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1337</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="G117" t="s">
+        <v>510</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>735</v>
+      </c>
+      <c r="B118" t="s">
+        <v>736</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D118" t="s">
+        <v>738</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1375</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="M118" s="2" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="129" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="130" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6751,9 +6986,38 @@
     <hyperlink ref="L13" r:id="rId340"/>
     <hyperlink ref="M13" r:id="rId341"/>
     <hyperlink ref="N13" r:id="rId342"/>
+    <hyperlink ref="J29" r:id="rId343"/>
+    <hyperlink ref="K29" r:id="rId344"/>
+    <hyperlink ref="L29" r:id="rId345"/>
+    <hyperlink ref="M29" r:id="rId346"/>
+    <hyperlink ref="J30" r:id="rId347"/>
+    <hyperlink ref="K30" r:id="rId348"/>
+    <hyperlink ref="L30" r:id="rId349"/>
+    <hyperlink ref="M30" r:id="rId350"/>
+    <hyperlink ref="J9" r:id="rId351"/>
+    <hyperlink ref="K9" r:id="rId352"/>
+    <hyperlink ref="L9" r:id="rId353"/>
+    <hyperlink ref="M9" r:id="rId354"/>
+    <hyperlink ref="J14" r:id="rId355"/>
+    <hyperlink ref="K14" r:id="rId356"/>
+    <hyperlink ref="L14" r:id="rId357"/>
+    <hyperlink ref="M14" r:id="rId358"/>
+    <hyperlink ref="H117" r:id="rId359"/>
+    <hyperlink ref="I117" r:id="rId360"/>
+    <hyperlink ref="J117" r:id="rId361"/>
+    <hyperlink ref="K117" r:id="rId362"/>
+    <hyperlink ref="L117" r:id="rId363"/>
+    <hyperlink ref="M117" r:id="rId364"/>
+    <hyperlink ref="C118" r:id="rId365"/>
+    <hyperlink ref="H118" r:id="rId366"/>
+    <hyperlink ref="I118" r:id="rId367"/>
+    <hyperlink ref="J118" r:id="rId368"/>
+    <hyperlink ref="K118" r:id="rId369"/>
+    <hyperlink ref="L118" r:id="rId370"/>
+    <hyperlink ref="M118" r:id="rId371"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId343"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId372"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add the life line
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/храмы.xlsx
+++ b/loadDatabase/religion/храмы.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="768">
   <si>
     <t>название</t>
   </si>
@@ -2324,9 +2324,6 @@
     <t>Собор Сошествия Святого Духа</t>
   </si>
   <si>
-    <t>Минкс</t>
-  </si>
-  <si>
     <t>53°54′18″ с. ш. 27°33′22″ в. д.</t>
   </si>
   <si>
@@ -2888,8 +2885,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3057,7 +3054,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3089,9 +3086,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3123,6 +3121,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3298,15 +3297,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.85546875" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
@@ -3315,7 +3314,7 @@
     <col min="9" max="9" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.95" customHeight="1">
+    <row r="1" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3344,22 +3343,22 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
+        <v>652</v>
+      </c>
+      <c r="K1" t="s">
         <v>653</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>654</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>655</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>656</v>
       </c>
-      <c r="N1" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="14" customFormat="1" ht="15.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:14" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>136</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>451</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E2" s="1">
         <v>1903</v>
@@ -3391,7 +3390,7 @@
       <c r="M2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" s="14" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="1:14" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>550</v>
       </c>
@@ -3425,7 +3424,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" ht="15.95" customHeight="1">
+    <row r="4" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -3433,7 +3432,7 @@
         <v>481</v>
       </c>
       <c r="D4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E4" s="1">
         <v>1222</v>
@@ -3451,7 +3450,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.95" customHeight="1">
+    <row r="5" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>520</v>
       </c>
@@ -3480,59 +3479,59 @@
         <v>514</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.95" customHeight="1">
+    <row r="6" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>520</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E6" s="1">
         <v>1761</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.95" customHeight="1">
+    </row>
+    <row r="7" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7" t="s">
+        <v>610</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D7" t="s">
         <v>609</v>
-      </c>
-      <c r="B7" t="s">
-        <v>611</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="D7" t="s">
-        <v>610</v>
       </c>
       <c r="E7" s="1">
         <v>1180</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.95" customHeight="1">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>370</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>372</v>
       </c>
       <c r="D8" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E8" s="1">
         <v>1259</v>
@@ -3558,7 +3557,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.95" customHeight="1">
+    <row r="9" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>326</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>494</v>
       </c>
       <c r="D9" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E9" s="1">
         <v>1676</v>
@@ -3584,19 +3583,19 @@
         <v>316</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.95" customHeight="1">
+    </row>
+    <row r="10" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>203</v>
       </c>
@@ -3621,7 +3620,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.95" customHeight="1">
+    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>272</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>482</v>
       </c>
       <c r="D11" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E11" s="1">
         <v>1230</v>
@@ -3644,7 +3643,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.95" customHeight="1">
+    <row r="12" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>479</v>
       </c>
       <c r="D12" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E12" s="1">
         <v>1194</v>
@@ -3667,7 +3666,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.95" customHeight="1">
+    <row r="13" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>526</v>
       </c>
@@ -3693,22 +3692,22 @@
         <v>514</v>
       </c>
       <c r="J13" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="K13" s="17" t="s">
         <v>658</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="L13" s="17" t="s">
         <v>659</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="M13" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="N13" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="N13" s="17" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.95" customHeight="1">
+    </row>
+    <row r="14" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>328</v>
       </c>
@@ -3719,7 +3718,7 @@
         <v>495</v>
       </c>
       <c r="D14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E14" s="1">
         <v>1677</v>
@@ -3734,19 +3733,19 @@
         <v>316</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.95" customHeight="1">
+    </row>
+    <row r="15" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>358</v>
       </c>
@@ -3757,7 +3756,7 @@
         <v>360</v>
       </c>
       <c r="D15" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E15" s="1">
         <v>1050</v>
@@ -3772,7 +3771,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.95" customHeight="1">
+    <row r="16" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -3799,7 +3798,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="15.95" customHeight="1">
+    <row r="17" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>292</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>487</v>
       </c>
       <c r="D17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E17" s="1">
         <v>1215</v>
@@ -3822,7 +3821,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.95" customHeight="1">
+    <row r="18" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -3848,7 +3847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.95" customHeight="1">
+    <row r="19" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>541</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.95" customHeight="1">
+    <row r="20" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.95" customHeight="1">
+    <row r="21" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>531</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.95" customHeight="1">
+    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>132</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>450</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E22" s="1">
         <v>1885</v>
@@ -3951,33 +3950,33 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.95" customHeight="1">
+    <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>620</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="D23" t="s">
         <v>622</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="D23" t="s">
-        <v>623</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.95" customHeight="1">
+    </row>
+    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>558</v>
       </c>
@@ -4006,33 +4005,33 @@
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.95" customHeight="1">
+    <row r="25" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>600</v>
+      </c>
+      <c r="B25" t="s">
+        <v>603</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D25" t="s">
         <v>601</v>
-      </c>
-      <c r="B25" t="s">
-        <v>604</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="D25" t="s">
-        <v>602</v>
       </c>
       <c r="E25" s="1">
         <v>1830</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.95" customHeight="1">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>334</v>
       </c>
@@ -4058,30 +4057,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.95" customHeight="1">
+    <row r="27" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>594</v>
+      </c>
+      <c r="B27" t="s">
+        <v>597</v>
+      </c>
+      <c r="C27" t="s">
+        <v>596</v>
+      </c>
+      <c r="D27" t="s">
         <v>595</v>
-      </c>
-      <c r="B27" t="s">
-        <v>598</v>
-      </c>
-      <c r="C27" t="s">
-        <v>597</v>
-      </c>
-      <c r="D27" t="s">
-        <v>596</v>
       </c>
       <c r="E27" s="1">
         <v>1861</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.95" customHeight="1">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>177</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>461</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E28" s="1">
         <v>1714</v>
@@ -4106,7 +4105,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.95" customHeight="1">
+    <row r="29" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>5</v>
       </c>
@@ -4115,7 +4114,7 @@
         <v>507</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E29" s="11">
         <v>1637</v>
@@ -4133,28 +4132,28 @@
         <v>9</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N29" s="14"/>
     </row>
-    <row r="30" spans="1:14" ht="15.95" customHeight="1">
+    <row r="30" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>313</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D30" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>538</v>
@@ -4172,45 +4171,45 @@
         <v>316</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>766</v>
-      </c>
       <c r="M30" s="2" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="15.95" customHeight="1">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>633</v>
+      </c>
+      <c r="B31" t="s">
         <v>634</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D31" t="s">
         <v>635</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="D31" t="s">
-        <v>636</v>
       </c>
       <c r="E31" s="1">
         <v>1825</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.95" customHeight="1">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.95" customHeight="1">
+    <row r="33" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.95" customHeight="1">
+    <row r="34" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>352</v>
       </c>
@@ -4267,7 +4266,7 @@
         <v>354</v>
       </c>
       <c r="D34" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E34" s="1">
         <v>960</v>
@@ -4282,7 +4281,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.95" customHeight="1">
+    <row r="35" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>341</v>
       </c>
@@ -4293,7 +4292,7 @@
         <v>343</v>
       </c>
       <c r="D35" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E35" s="1">
         <v>323</v>
@@ -4308,7 +4307,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.95" customHeight="1">
+    <row r="36" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>419</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>421</v>
       </c>
       <c r="D36" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E36" s="1">
         <v>2004</v>
@@ -4334,7 +4333,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.95" customHeight="1">
+    <row r="37" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>347</v>
       </c>
@@ -4342,10 +4341,10 @@
         <v>348</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D37" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E37" s="1">
         <v>1590</v>
@@ -4360,33 +4359,33 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.95" customHeight="1">
+    <row r="38" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>581</v>
       </c>
       <c r="B38" t="s">
+        <v>582</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>584</v>
-      </c>
       <c r="D38" t="s">
-        <v>582</v>
+        <v>644</v>
       </c>
       <c r="E38" s="1">
         <v>1633</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.95" customHeight="1">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -4409,7 +4408,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.95" customHeight="1">
+    <row r="40" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>376</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>378</v>
       </c>
       <c r="D40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E40" s="1">
         <v>537</v>
@@ -4435,7 +4434,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.95" customHeight="1">
+    <row r="41" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>566</v>
       </c>
@@ -4464,15 +4463,15 @@
         <v>570</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.95" customHeight="1">
+    <row r="42" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E42" s="1">
         <v>2002</v>
@@ -4487,33 +4486,33 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.95" customHeight="1">
+    <row r="43" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>639</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>642</v>
-      </c>
       <c r="D43" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E43" s="1">
         <v>1195</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>644</v>
-      </c>
       <c r="I43" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.95" customHeight="1">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>574</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.95" customHeight="1">
+    <row r="45" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -4547,7 +4546,7 @@
         <v>478</v>
       </c>
       <c r="D45" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E45" s="1">
         <v>1161</v>
@@ -4565,7 +4564,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.95" customHeight="1">
+    <row r="46" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>509</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.95" customHeight="1">
+    <row r="47" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>248</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>249</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>250</v>
@@ -4616,7 +4615,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.95" customHeight="1">
+    <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -4624,7 +4623,7 @@
         <v>488</v>
       </c>
       <c r="D48" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E48" s="1">
         <v>1657</v>
@@ -4639,7 +4638,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15.95" customHeight="1">
+    <row r="49" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>12</v>
       </c>
@@ -4669,7 +4668,7 @@
       <c r="M49" s="14"/>
       <c r="N49" s="14"/>
     </row>
-    <row r="50" spans="1:14" ht="15.95" customHeight="1">
+    <row r="50" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15.95" customHeight="1">
+    <row r="51" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -4719,7 +4718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15.95" customHeight="1">
+    <row r="52" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>317</v>
       </c>
@@ -4727,7 +4726,7 @@
         <v>492</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E52" s="1">
         <v>1690</v>
@@ -4745,7 +4744,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.95" customHeight="1">
+    <row r="53" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>185</v>
       </c>
@@ -4754,7 +4753,7 @@
         <v>463</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E53" s="1">
         <v>1906</v>
@@ -4770,7 +4769,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.95" customHeight="1">
+    <row r="54" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>322</v>
       </c>
@@ -4779,7 +4778,7 @@
         <v>493</v>
       </c>
       <c r="D54" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E54" s="1">
         <v>1870</v>
@@ -4797,7 +4796,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15.95" customHeight="1">
+    <row r="55" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>197</v>
       </c>
@@ -4824,7 +4823,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15.95" customHeight="1">
+    <row r="56" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15.95" customHeight="1">
+    <row r="57" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -4870,7 +4869,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15.95" customHeight="1">
+    <row r="58" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>237</v>
       </c>
@@ -4882,7 +4881,7 @@
         <v>238</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>239</v>
@@ -4897,7 +4896,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15.95" customHeight="1">
+    <row r="59" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -4908,7 +4907,7 @@
         <v>30</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F59" t="s">
         <v>31</v>
@@ -4920,7 +4919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15.95" customHeight="1">
+    <row r="60" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>189</v>
       </c>
@@ -4929,7 +4928,7 @@
         <v>464</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E60" s="1">
         <v>1860</v>
@@ -4945,7 +4944,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15.95" customHeight="1">
+    <row r="61" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>516</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15.95" customHeight="1">
+    <row r="62" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15.95" customHeight="1">
+    <row r="63" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15.95" customHeight="1">
+    <row r="64" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -5040,7 +5039,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.95" customHeight="1">
+    <row r="65" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -5063,41 +5062,41 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.95" customHeight="1">
+    <row r="66" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>587</v>
+      </c>
+      <c r="B66" t="s">
+        <v>589</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="B66" t="s">
-        <v>590</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>589</v>
-      </c>
       <c r="D66" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E66" s="1">
         <v>1994</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G66" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.95" customHeight="1">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>21</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>22</v>
@@ -5118,7 +5117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.95" customHeight="1">
+    <row r="68" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -5126,7 +5125,7 @@
         <v>444</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E68" s="1">
         <v>1955</v>
@@ -5141,7 +5140,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.95" customHeight="1">
+    <row r="69" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -5149,7 +5148,7 @@
         <v>446</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E69" s="1">
         <v>1872</v>
@@ -5164,7 +5163,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.95" customHeight="1">
+    <row r="70" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>101</v>
       </c>
@@ -5173,10 +5172,10 @@
         <v>474</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>233</v>
@@ -5191,12 +5190,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.95" customHeight="1">
+    <row r="71" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>110</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>111</v>
@@ -5214,7 +5213,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.95" customHeight="1">
+    <row r="72" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>149</v>
       </c>
@@ -5223,7 +5222,7 @@
         <v>454</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E72" s="1">
         <v>2018</v>
@@ -5239,7 +5238,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.95" customHeight="1">
+    <row r="73" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>118</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.95" customHeight="1">
+    <row r="74" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>262</v>
       </c>
@@ -5285,7 +5284,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.95" customHeight="1">
+    <row r="75" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>280</v>
       </c>
@@ -5293,7 +5292,7 @@
         <v>484</v>
       </c>
       <c r="D75" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E75" s="1">
         <v>1571</v>
@@ -5308,7 +5307,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.95" customHeight="1">
+    <row r="76" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>243</v>
       </c>
@@ -5320,7 +5319,7 @@
         <v>244</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>245</v>
@@ -5333,7 +5332,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.95" customHeight="1">
+    <row r="77" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>123</v>
       </c>
@@ -5341,7 +5340,7 @@
         <v>448</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E77" s="1">
         <v>1918</v>
@@ -5356,7 +5355,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.95" customHeight="1">
+    <row r="78" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>34</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.95" customHeight="1">
+    <row r="79" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>145</v>
       </c>
@@ -5388,7 +5387,7 @@
         <v>453</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E79" s="1">
         <v>1896</v>
@@ -5404,7 +5403,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.95" customHeight="1">
+    <row r="80" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>46</v>
       </c>
@@ -5427,7 +5426,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.95" customHeight="1">
+    <row r="81" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>169</v>
       </c>
@@ -5436,7 +5435,7 @@
         <v>459</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E81" s="1">
         <v>2002</v>
@@ -5452,7 +5451,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.95" customHeight="1">
+    <row r="82" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>30</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>68</v>
@@ -5475,7 +5474,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.95" customHeight="1">
+    <row r="83" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>214</v>
       </c>
@@ -5484,10 +5483,10 @@
         <v>469</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>213</v>
@@ -5500,7 +5499,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.95" customHeight="1">
+    <row r="84" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>214</v>
       </c>
@@ -5508,10 +5507,10 @@
         <v>382</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D84" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>537</v>
@@ -5526,7 +5525,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.95" customHeight="1">
+    <row r="85" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>173</v>
       </c>
@@ -5535,7 +5534,7 @@
         <v>460</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E85" s="1">
         <v>2001</v>
@@ -5551,7 +5550,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.95" customHeight="1">
+    <row r="86" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>221</v>
       </c>
@@ -5560,10 +5559,10 @@
         <v>471</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>222</v>
@@ -5576,7 +5575,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.95" customHeight="1">
+    <row r="87" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>276</v>
       </c>
@@ -5584,7 +5583,7 @@
         <v>483</v>
       </c>
       <c r="D87" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E87" s="1">
         <v>1555</v>
@@ -5599,7 +5598,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.95" customHeight="1">
+    <row r="88" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>64</v>
       </c>
@@ -5622,7 +5621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.95" customHeight="1">
+    <row r="89" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>386</v>
       </c>
@@ -5633,7 +5632,7 @@
         <v>388</v>
       </c>
       <c r="D89" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>536</v>
@@ -5648,7 +5647,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.95" customHeight="1">
+    <row r="90" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>386</v>
       </c>
@@ -5659,7 +5658,7 @@
         <v>415</v>
       </c>
       <c r="D90" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E90" s="1">
         <v>1380</v>
@@ -5674,7 +5673,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.95" customHeight="1">
+    <row r="91" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>27</v>
       </c>
@@ -5682,7 +5681,7 @@
         <v>500</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
@@ -5697,7 +5696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.95" customHeight="1">
+    <row r="92" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>284</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>485</v>
       </c>
       <c r="D92" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E92" s="1">
         <v>1650</v>
@@ -5720,7 +5719,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15.95" customHeight="1">
+    <row r="93" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>408</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>410</v>
       </c>
       <c r="D93" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E93" s="1">
         <v>1295</v>
@@ -5746,7 +5745,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.95" customHeight="1">
+    <row r="94" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>193</v>
       </c>
@@ -5755,7 +5754,7 @@
         <v>465</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E94" s="1">
         <v>2018</v>
@@ -5771,7 +5770,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.95" customHeight="1">
+    <row r="95" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>304</v>
       </c>
@@ -5779,7 +5778,7 @@
         <v>490</v>
       </c>
       <c r="D95" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E95" s="1">
         <v>1665</v>
@@ -5794,7 +5793,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15.95" customHeight="1">
+    <row r="96" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>300</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>489</v>
       </c>
       <c r="D96" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E96" s="1">
         <v>1620</v>
@@ -5817,7 +5816,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.95" customHeight="1">
+    <row r="97" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>229</v>
       </c>
@@ -5826,10 +5825,10 @@
         <v>473</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>230</v>
@@ -5842,7 +5841,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.95" customHeight="1">
+    <row r="98" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>153</v>
       </c>
@@ -5851,7 +5850,7 @@
         <v>455</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E98" s="1">
         <v>1838</v>
@@ -5867,7 +5866,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.95" customHeight="1">
+    <row r="99" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>141</v>
       </c>
@@ -5876,7 +5875,7 @@
         <v>452</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>539</v>
@@ -5892,7 +5891,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.95" customHeight="1">
+    <row r="100" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>165</v>
       </c>
@@ -5901,7 +5900,7 @@
         <v>458</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E100" s="1">
         <v>1817</v>
@@ -5917,7 +5916,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.95" customHeight="1">
+    <row r="101" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>157</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>456</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E101" s="1">
         <v>1888</v>
@@ -5942,7 +5941,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.95" customHeight="1">
+    <row r="102" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>161</v>
       </c>
@@ -5951,7 +5950,7 @@
         <v>457</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E102" s="1">
         <v>1857</v>
@@ -5967,7 +5966,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15.95" customHeight="1">
+    <row r="103" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>208</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.95" customHeight="1">
+    <row r="104" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>225</v>
       </c>
@@ -6001,10 +6000,10 @@
         <v>472</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>226</v>
@@ -6017,7 +6016,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.95" customHeight="1">
+    <row r="105" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>181</v>
       </c>
@@ -6026,7 +6025,7 @@
         <v>462</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E105" s="1">
         <v>1855</v>
@@ -6042,7 +6041,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.95" customHeight="1">
+    <row r="106" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>217</v>
       </c>
@@ -6051,10 +6050,10 @@
         <v>470</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>218</v>
@@ -6067,7 +6066,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.95" customHeight="1">
+    <row r="107" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>288</v>
       </c>
@@ -6075,7 +6074,7 @@
         <v>486</v>
       </c>
       <c r="D107" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E107" s="1">
         <v>1691</v>
@@ -6090,7 +6089,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.95" customHeight="1">
+    <row r="108" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>127</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.95" customHeight="1">
+    <row r="109" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>127</v>
       </c>
@@ -6145,7 +6144,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.95" customHeight="1">
+    <row r="110" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>364</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15.95" customHeight="1">
+    <row r="111" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>397</v>
       </c>
@@ -6179,7 +6178,7 @@
         <v>399</v>
       </c>
       <c r="D111" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E111" s="1">
         <v>1306</v>
@@ -6194,7 +6193,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15.95" customHeight="1">
+    <row r="112" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>308</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>491</v>
       </c>
       <c r="D112" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E112" s="1">
         <v>1695</v>
@@ -6217,7 +6216,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="15.95" customHeight="1">
+    <row r="113" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>403</v>
       </c>
@@ -6237,7 +6236,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="15.95" customHeight="1">
+    <row r="114" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>392</v>
       </c>
@@ -6245,10 +6244,10 @@
         <v>393</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D114" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E114" s="1">
         <v>1230</v>
@@ -6263,7 +6262,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="15.95" customHeight="1">
+    <row r="115" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -6283,508 +6282,508 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="15.95" customHeight="1">
+    <row r="116" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>628</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>631</v>
-      </c>
       <c r="D116" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E116" s="1">
         <v>2004</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="15.95" customHeight="1">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>705</v>
+      </c>
+      <c r="B117" t="s">
         <v>706</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>707</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>708</v>
-      </c>
-      <c r="D117" t="s">
-        <v>709</v>
       </c>
       <c r="E117" s="1">
         <v>1337</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G117" t="s">
         <v>508</v>
       </c>
       <c r="H117" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="I117" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="J117" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="K117" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="K117" s="2" t="s">
+      <c r="L117" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="L117" s="2" t="s">
+      <c r="M117" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="M117" s="2" t="s">
+    </row>
+    <row r="118" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" ht="15.95" customHeight="1">
-      <c r="A118" t="s">
+      <c r="B118" t="s">
         <v>717</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="D118" t="s">
         <v>719</v>
-      </c>
-      <c r="D118" t="s">
-        <v>720</v>
       </c>
       <c r="E118" s="1">
         <v>1375</v>
       </c>
       <c r="F118" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="H118" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="I118" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="J118" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="J118" s="2" t="s">
+      <c r="K118" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="K118" s="2" t="s">
+      <c r="L118" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="M118" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="M118" s="2" t="s">
+    </row>
+    <row r="119" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" ht="15.95" customHeight="1">
-      <c r="A119" t="s">
+      <c r="B119" t="s">
         <v>728</v>
       </c>
-      <c r="B119" t="s">
-        <v>729</v>
-      </c>
       <c r="C119" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D119" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E119" s="1">
         <v>1215</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G119" t="s">
+        <v>729</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="I119" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="H119" s="2" t="s">
-        <v>732</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>731</v>
-      </c>
       <c r="J119" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="N119" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="K119" s="2" t="s">
+    </row>
+    <row r="120" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>739</v>
       </c>
-      <c r="L119" s="2" t="s">
-        <v>738</v>
-      </c>
-      <c r="M119" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="N119" s="2" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" ht="15.95" customHeight="1">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>740</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="D120" t="s">
         <v>742</v>
-      </c>
-      <c r="D120" t="s">
-        <v>743</v>
       </c>
       <c r="E120" s="1">
         <v>324</v>
       </c>
       <c r="F120" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="N120" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="H120" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="L120" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="M120" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="N120" s="2" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="122" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="123" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="124" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="125" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="126" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="127" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="128" spans="1:14" ht="15.95" customHeight="1"/>
-    <row r="129" ht="15.95" customHeight="1"/>
-    <row r="130" ht="15.95" customHeight="1"/>
-    <row r="131" ht="15.95" customHeight="1"/>
-    <row r="132" ht="15.95" customHeight="1"/>
-    <row r="133" ht="15.95" customHeight="1"/>
-    <row r="134" ht="15.95" customHeight="1"/>
-    <row r="135" ht="15.95" customHeight="1"/>
-    <row r="136" ht="15.95" customHeight="1"/>
-    <row r="137" ht="15.95" customHeight="1"/>
-    <row r="138" ht="15.95" customHeight="1"/>
-    <row r="139" ht="15.95" customHeight="1"/>
-    <row r="140" ht="15.95" customHeight="1"/>
-    <row r="141" ht="15.95" customHeight="1"/>
-    <row r="142" ht="15.95" customHeight="1"/>
-    <row r="143" ht="15.95" customHeight="1"/>
-    <row r="144" ht="15.95" customHeight="1"/>
-    <row r="145" ht="15.95" customHeight="1"/>
-    <row r="146" ht="15.95" customHeight="1"/>
-    <row r="147" ht="15.95" customHeight="1"/>
-    <row r="148" ht="15.95" customHeight="1"/>
-    <row r="149" ht="15.95" customHeight="1"/>
-    <row r="150" ht="15.95" customHeight="1"/>
-    <row r="151" ht="15.95" customHeight="1"/>
-    <row r="152" ht="15.95" customHeight="1"/>
-    <row r="153" ht="15.95" customHeight="1"/>
-    <row r="154" ht="15.95" customHeight="1"/>
-    <row r="155" ht="15.95" customHeight="1"/>
-    <row r="156" ht="15.95" customHeight="1"/>
-    <row r="157" ht="15.95" customHeight="1"/>
-    <row r="158" ht="15.95" customHeight="1"/>
-    <row r="159" ht="15.95" customHeight="1"/>
-    <row r="160" ht="15.95" customHeight="1"/>
-    <row r="161" ht="15.95" customHeight="1"/>
-    <row r="162" ht="15.95" customHeight="1"/>
-    <row r="163" ht="15.95" customHeight="1"/>
-    <row r="164" ht="15.95" customHeight="1"/>
-    <row r="165" ht="15.95" customHeight="1"/>
-    <row r="166" ht="15.95" customHeight="1"/>
-    <row r="167" ht="15.95" customHeight="1"/>
-    <row r="168" ht="15.95" customHeight="1"/>
-    <row r="169" ht="15.95" customHeight="1"/>
-    <row r="170" ht="15.95" customHeight="1"/>
-    <row r="171" ht="15.95" customHeight="1"/>
-    <row r="172" ht="15.95" customHeight="1"/>
-    <row r="173" ht="15.95" customHeight="1"/>
-    <row r="174" ht="15.95" customHeight="1"/>
-    <row r="175" ht="15.95" customHeight="1"/>
-    <row r="176" ht="15.95" customHeight="1"/>
-    <row r="177" ht="15.95" customHeight="1"/>
-    <row r="178" ht="15.95" customHeight="1"/>
-    <row r="179" ht="15.95" customHeight="1"/>
-    <row r="180" ht="15.95" customHeight="1"/>
-    <row r="181" ht="15.95" customHeight="1"/>
-    <row r="182" ht="15.95" customHeight="1"/>
-    <row r="183" ht="15.95" customHeight="1"/>
-    <row r="184" ht="15.95" customHeight="1"/>
-    <row r="185" ht="15.95" customHeight="1"/>
-    <row r="186" ht="15.95" customHeight="1"/>
-    <row r="187" ht="15.95" customHeight="1"/>
-    <row r="188" ht="15.95" customHeight="1"/>
-    <row r="189" ht="15.95" customHeight="1"/>
-    <row r="190" ht="15.95" customHeight="1"/>
-    <row r="191" ht="15.95" customHeight="1"/>
-    <row r="192" ht="15.95" customHeight="1"/>
-    <row r="193" ht="15.95" customHeight="1"/>
-    <row r="194" ht="15.95" customHeight="1"/>
-    <row r="195" ht="15.95" customHeight="1"/>
-    <row r="196" ht="15.95" customHeight="1"/>
-    <row r="197" ht="15.95" customHeight="1"/>
-    <row r="198" ht="15.95" customHeight="1"/>
-    <row r="199" ht="15.95" customHeight="1"/>
-    <row r="200" ht="15.95" customHeight="1"/>
-    <row r="201" ht="15.95" customHeight="1"/>
-    <row r="202" ht="15.95" customHeight="1"/>
-    <row r="203" ht="15.95" customHeight="1"/>
-    <row r="204" ht="15.95" customHeight="1"/>
-    <row r="205" ht="15.95" customHeight="1"/>
-    <row r="206" ht="15.95" customHeight="1"/>
-    <row r="207" ht="15.95" customHeight="1"/>
-    <row r="208" ht="15.95" customHeight="1"/>
-    <row r="209" ht="15.95" customHeight="1"/>
-    <row r="210" ht="15.95" customHeight="1"/>
-    <row r="211" ht="15.95" customHeight="1"/>
-    <row r="212" ht="15.95" customHeight="1"/>
-    <row r="213" ht="15.95" customHeight="1"/>
-    <row r="214" ht="15.95" customHeight="1"/>
-    <row r="215" ht="15.95" customHeight="1"/>
-    <row r="216" ht="15.95" customHeight="1"/>
-    <row r="217" ht="15.95" customHeight="1"/>
-    <row r="218" ht="15.95" customHeight="1"/>
-    <row r="219" ht="15.95" customHeight="1"/>
-    <row r="220" ht="15.95" customHeight="1"/>
-    <row r="221" ht="15.95" customHeight="1"/>
-    <row r="222" ht="15.95" customHeight="1"/>
-    <row r="223" ht="15.95" customHeight="1"/>
-    <row r="224" ht="15.95" customHeight="1"/>
-    <row r="225" ht="15.95" customHeight="1"/>
-    <row r="226" ht="15.95" customHeight="1"/>
-    <row r="227" ht="15.95" customHeight="1"/>
-    <row r="228" ht="15.95" customHeight="1"/>
-    <row r="229" ht="15.95" customHeight="1"/>
-    <row r="230" ht="15.95" customHeight="1"/>
-    <row r="231" ht="15.95" customHeight="1"/>
-    <row r="232" ht="15.95" customHeight="1"/>
-    <row r="233" ht="15.95" customHeight="1"/>
-    <row r="234" ht="15.95" customHeight="1"/>
-    <row r="235" ht="15.95" customHeight="1"/>
-    <row r="236" ht="15.95" customHeight="1"/>
-    <row r="237" ht="15.95" customHeight="1"/>
-    <row r="238" ht="15.95" customHeight="1"/>
-    <row r="239" ht="15.95" customHeight="1"/>
-    <row r="240" ht="15.95" customHeight="1"/>
-    <row r="241" ht="15.95" customHeight="1"/>
-    <row r="242" ht="15.95" customHeight="1"/>
-    <row r="243" ht="15.95" customHeight="1"/>
-    <row r="244" ht="15.95" customHeight="1"/>
-    <row r="245" ht="15.95" customHeight="1"/>
-    <row r="246" ht="15.95" customHeight="1"/>
-    <row r="247" ht="15.95" customHeight="1"/>
-    <row r="248" ht="15.95" customHeight="1"/>
-    <row r="249" ht="15.95" customHeight="1"/>
-    <row r="250" ht="15.95" customHeight="1"/>
-    <row r="251" ht="15.95" customHeight="1"/>
-    <row r="252" ht="15.95" customHeight="1"/>
-    <row r="253" ht="15.95" customHeight="1"/>
-    <row r="254" ht="15.95" customHeight="1"/>
-    <row r="255" ht="15.95" customHeight="1"/>
-    <row r="256" ht="15.95" customHeight="1"/>
-    <row r="257" ht="15.95" customHeight="1"/>
-    <row r="258" ht="15.95" customHeight="1"/>
-    <row r="259" ht="15.95" customHeight="1"/>
-    <row r="260" ht="15.95" customHeight="1"/>
-    <row r="261" ht="15.95" customHeight="1"/>
-    <row r="262" ht="15.95" customHeight="1"/>
-    <row r="263" ht="15.95" customHeight="1"/>
-    <row r="264" ht="15.95" customHeight="1"/>
-    <row r="265" ht="15.95" customHeight="1"/>
-    <row r="266" ht="15.95" customHeight="1"/>
-    <row r="267" ht="15.95" customHeight="1"/>
-    <row r="268" ht="15.95" customHeight="1"/>
-    <row r="269" ht="15.95" customHeight="1"/>
-    <row r="270" ht="15.95" customHeight="1"/>
-    <row r="271" ht="15.95" customHeight="1"/>
-    <row r="272" ht="15.95" customHeight="1"/>
-    <row r="273" ht="15.95" customHeight="1"/>
-    <row r="274" ht="15.95" customHeight="1"/>
-    <row r="275" ht="15.95" customHeight="1"/>
-    <row r="276" ht="15.95" customHeight="1"/>
-    <row r="277" ht="15.95" customHeight="1"/>
-    <row r="278" ht="15.95" customHeight="1"/>
-    <row r="279" ht="15.95" customHeight="1"/>
-    <row r="280" ht="15.95" customHeight="1"/>
-    <row r="281" ht="15.95" customHeight="1"/>
-    <row r="282" ht="15.95" customHeight="1"/>
-    <row r="283" ht="15.95" customHeight="1"/>
-    <row r="284" ht="15.95" customHeight="1"/>
-    <row r="285" ht="15.95" customHeight="1"/>
-    <row r="286" ht="15.95" customHeight="1"/>
-    <row r="287" ht="15.95" customHeight="1"/>
-    <row r="288" ht="15.95" customHeight="1"/>
-    <row r="289" ht="15.95" customHeight="1"/>
-    <row r="290" ht="15.95" customHeight="1"/>
-    <row r="291" ht="15.95" customHeight="1"/>
-    <row r="292" ht="15.95" customHeight="1"/>
-    <row r="293" ht="15.95" customHeight="1"/>
-    <row r="294" ht="15.95" customHeight="1"/>
-    <row r="295" ht="15.95" customHeight="1"/>
-    <row r="296" ht="15.95" customHeight="1"/>
-    <row r="297" ht="15.95" customHeight="1"/>
-    <row r="298" ht="15.95" customHeight="1"/>
-    <row r="299" ht="15.95" customHeight="1"/>
-    <row r="300" ht="15.95" customHeight="1"/>
-    <row r="301" ht="15.95" customHeight="1"/>
-    <row r="302" ht="15.95" customHeight="1"/>
-    <row r="303" ht="15.95" customHeight="1"/>
-    <row r="304" ht="15.95" customHeight="1"/>
-    <row r="305" ht="15.95" customHeight="1"/>
-    <row r="306" ht="15.95" customHeight="1"/>
-    <row r="307" ht="15.95" customHeight="1"/>
-    <row r="308" ht="15.95" customHeight="1"/>
-    <row r="309" ht="15.95" customHeight="1"/>
-    <row r="310" ht="15.95" customHeight="1"/>
-    <row r="311" ht="15.95" customHeight="1"/>
-    <row r="312" ht="15.95" customHeight="1"/>
-    <row r="313" ht="15.95" customHeight="1"/>
-    <row r="314" ht="15.95" customHeight="1"/>
-    <row r="315" ht="15.95" customHeight="1"/>
-    <row r="316" ht="15.95" customHeight="1"/>
-    <row r="317" ht="15.95" customHeight="1"/>
-    <row r="318" ht="15.95" customHeight="1"/>
-    <row r="319" ht="15.95" customHeight="1"/>
-    <row r="320" ht="15.95" customHeight="1"/>
-    <row r="321" ht="15.95" customHeight="1"/>
-    <row r="322" ht="15.95" customHeight="1"/>
-    <row r="323" ht="15.95" customHeight="1"/>
-    <row r="324" ht="15.95" customHeight="1"/>
-    <row r="325" ht="15.95" customHeight="1"/>
-    <row r="326" ht="15.95" customHeight="1"/>
-    <row r="327" ht="15.95" customHeight="1"/>
-    <row r="328" ht="15.95" customHeight="1"/>
-    <row r="329" ht="15.95" customHeight="1"/>
-    <row r="330" ht="15.95" customHeight="1"/>
-    <row r="331" ht="15.95" customHeight="1"/>
-    <row r="332" ht="15.95" customHeight="1"/>
-    <row r="333" ht="15.95" customHeight="1"/>
-    <row r="334" ht="15.95" customHeight="1"/>
-    <row r="335" ht="15.95" customHeight="1"/>
-    <row r="336" ht="15.95" customHeight="1"/>
-    <row r="337" ht="15.95" customHeight="1"/>
-    <row r="338" ht="15.95" customHeight="1"/>
-    <row r="339" ht="15.95" customHeight="1"/>
-    <row r="340" ht="15.95" customHeight="1"/>
-    <row r="341" ht="15.95" customHeight="1"/>
-    <row r="342" ht="15.95" customHeight="1"/>
-    <row r="343" ht="15.95" customHeight="1"/>
-    <row r="344" ht="15.95" customHeight="1"/>
-    <row r="345" ht="15.95" customHeight="1"/>
-    <row r="346" ht="15.95" customHeight="1"/>
-    <row r="347" ht="15.95" customHeight="1"/>
-    <row r="348" ht="15.95" customHeight="1"/>
-    <row r="349" ht="15.95" customHeight="1"/>
-    <row r="350" ht="15.95" customHeight="1"/>
-    <row r="351" ht="15.95" customHeight="1"/>
-    <row r="352" ht="15.95" customHeight="1"/>
-    <row r="353" ht="15.95" customHeight="1"/>
-    <row r="354" ht="15.95" customHeight="1"/>
-    <row r="355" ht="15.95" customHeight="1"/>
-    <row r="356" ht="15.95" customHeight="1"/>
-    <row r="357" ht="15.95" customHeight="1"/>
-    <row r="358" ht="15.95" customHeight="1"/>
-    <row r="359" ht="15.95" customHeight="1"/>
-    <row r="360" ht="15.95" customHeight="1"/>
-    <row r="361" ht="15.95" customHeight="1"/>
-    <row r="362" ht="15.95" customHeight="1"/>
-    <row r="363" ht="15.95" customHeight="1"/>
-    <row r="364" ht="15.95" customHeight="1"/>
-    <row r="365" ht="15.95" customHeight="1"/>
-    <row r="366" ht="15.95" customHeight="1"/>
-    <row r="367" ht="15.95" customHeight="1"/>
-    <row r="368" ht="15.95" customHeight="1"/>
-    <row r="369" ht="15.95" customHeight="1"/>
-    <row r="370" ht="15.95" customHeight="1"/>
-    <row r="371" ht="15.95" customHeight="1"/>
-    <row r="372" ht="15.95" customHeight="1"/>
-    <row r="373" ht="15.95" customHeight="1"/>
-    <row r="374" ht="15.95" customHeight="1"/>
-    <row r="375" ht="15.95" customHeight="1"/>
-    <row r="376" ht="15.95" customHeight="1"/>
-    <row r="377" ht="15.95" customHeight="1"/>
-    <row r="378" ht="15.95" customHeight="1"/>
-    <row r="379" ht="15.95" customHeight="1"/>
-    <row r="380" ht="15.95" customHeight="1"/>
-    <row r="381" ht="15.95" customHeight="1"/>
-    <row r="382" ht="15.95" customHeight="1"/>
-    <row r="383" ht="15.95" customHeight="1"/>
-    <row r="384" ht="15.95" customHeight="1"/>
-    <row r="385" ht="15.95" customHeight="1"/>
-    <row r="386" ht="15.95" customHeight="1"/>
-    <row r="387" ht="15.95" customHeight="1"/>
-    <row r="388" ht="15.95" customHeight="1"/>
-    <row r="389" ht="15.95" customHeight="1"/>
-    <row r="390" ht="15.95" customHeight="1"/>
-    <row r="391" ht="15.95" customHeight="1"/>
-    <row r="392" ht="15.95" customHeight="1"/>
-    <row r="393" ht="15.95" customHeight="1"/>
-    <row r="394" ht="15.95" customHeight="1"/>
-    <row r="395" ht="15.95" customHeight="1"/>
-    <row r="396" ht="15.95" customHeight="1"/>
-    <row r="397" ht="15.95" customHeight="1"/>
-    <row r="398" ht="15.95" customHeight="1"/>
-    <row r="399" ht="15.95" customHeight="1"/>
-    <row r="400" ht="15.95" customHeight="1"/>
-    <row r="401" ht="15.95" customHeight="1"/>
-    <row r="402" ht="15.95" customHeight="1"/>
-    <row r="403" ht="15.95" customHeight="1"/>
-    <row r="404" ht="15.95" customHeight="1"/>
-    <row r="405" ht="15.95" customHeight="1"/>
-    <row r="406" ht="15.95" customHeight="1"/>
-    <row r="407" ht="15.95" customHeight="1"/>
-    <row r="408" ht="15.95" customHeight="1"/>
-    <row r="409" ht="15.95" customHeight="1"/>
-    <row r="410" ht="15.95" customHeight="1"/>
-    <row r="411" ht="15.95" customHeight="1"/>
-    <row r="412" ht="15.95" customHeight="1"/>
-    <row r="413" ht="15.95" customHeight="1"/>
-    <row r="414" ht="15.95" customHeight="1"/>
-    <row r="415" ht="15.95" customHeight="1"/>
-    <row r="416" ht="15.95" customHeight="1"/>
-    <row r="417" ht="15.95" customHeight="1"/>
-    <row r="418" ht="15.95" customHeight="1"/>
-    <row r="419" ht="15.95" customHeight="1"/>
-    <row r="420" ht="15.95" customHeight="1"/>
-    <row r="421" ht="15.95" customHeight="1"/>
-    <row r="422" ht="15.95" customHeight="1"/>
-    <row r="423" ht="15.95" customHeight="1"/>
-    <row r="424" ht="15.95" customHeight="1"/>
-    <row r="425" ht="15.95" customHeight="1"/>
-    <row r="426" ht="15.95" customHeight="1"/>
-    <row r="427" ht="15.95" customHeight="1"/>
-    <row r="428" ht="15.95" customHeight="1"/>
-    <row r="429" ht="15.95" customHeight="1"/>
-    <row r="430" ht="15.95" customHeight="1"/>
-    <row r="431" ht="15.95" customHeight="1"/>
-    <row r="432" ht="15.95" customHeight="1"/>
-    <row r="433" ht="15.95" customHeight="1"/>
-    <row r="434" ht="15.95" customHeight="1"/>
-    <row r="435" ht="15.95" customHeight="1"/>
+    </row>
+    <row r="121" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:N120">
     <sortState ref="A2:N116">
@@ -7185,19 +7184,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7220,135 +7219,135 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1">
+    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A4" s="17" t="s">
+    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A5" s="17" t="s">
+    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A6" s="17" t="s">
+    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A7" s="17" t="s">
+    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A8" s="17" t="s">
+    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A9" s="17" t="s">
+    <row r="10" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A10" s="17" t="s">
+    <row r="11" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A11" s="17" t="s">
+    <row r="12" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A12" s="17" t="s">
+    <row r="13" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A13" s="17" t="s">
+    <row r="14" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A14" s="17" t="s">
+    <row r="15" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A15" s="17" t="s">
+    <row r="16" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A16" s="17" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="18" spans="1:14" ht="18.95" customHeight="1">
+    <row r="17" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>658</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="17" t="s">
         <v>659</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="D18" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="F18" s="17" t="s">
         <v>662</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="G18" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="H18" s="17" t="s">
         <v>664</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="I18" s="17" t="s">
         <v>665</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="J18" s="17" t="s">
         <v>666</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="K18" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="L18" s="17" t="s">
         <v>668</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="M18" s="17" t="s">
         <v>669</v>
       </c>
-      <c r="M18" s="17" t="s">
+      <c r="N18" s="17" t="s">
         <v>670</v>
       </c>
-      <c r="N18" s="17" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="20" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="21" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="22" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="23" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="24" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="25" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="26" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="27" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="28" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="29" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="30" spans="1:14" ht="18.95" customHeight="1"/>
-    <row r="31" spans="1:14" ht="18.95" customHeight="1"/>
+    </row>
+    <row r="19" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -7386,19 +7385,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7421,16 +7420,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="10" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="11" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -7438,20 +7437,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7474,14 +7473,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="3" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="4" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="5" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="6" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="7" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="8" spans="1:7" ht="18.95" customHeight="1"/>
-    <row r="9" spans="1:7" ht="18.95" customHeight="1"/>
+    <row r="2" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>